<commit_message>
Integrate more tables in database
</commit_message>
<xml_diff>
--- a/Database Schema/Shopping_Database.xlsx
+++ b/Database Schema/Shopping_Database.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\eShoppingAdmin\Database Schema\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A8F339B3-870D-4026-BED6-0196B68AC749}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{467B0103-3689-41ED-8627-EB4810D2B7D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{23AB6FBB-2C3C-4DC6-A36A-5E0C15916A1A}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="925" uniqueCount="182">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="929" uniqueCount="184">
   <si>
     <t>Users</t>
   </si>
@@ -582,6 +582,12 @@
   </si>
   <si>
     <t>ProductImageURL</t>
+  </si>
+  <si>
+    <t>ProductPrice</t>
+  </si>
+  <si>
+    <t>SubCategoryId</t>
   </si>
 </sst>
 </file>
@@ -803,6 +809,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -823,10 +833,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1168,31 +1174,31 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:20" ht="18" x14ac:dyDescent="0.35">
-      <c r="B3" s="12" t="s">
+      <c r="B3" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="13"/>
-      <c r="D3" s="14"/>
-      <c r="F3" s="12" t="s">
+      <c r="C3" s="15"/>
+      <c r="D3" s="16"/>
+      <c r="F3" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="G3" s="13"/>
-      <c r="H3" s="14"/>
-      <c r="J3" s="12" t="s">
+      <c r="G3" s="15"/>
+      <c r="H3" s="16"/>
+      <c r="J3" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="K3" s="13"/>
-      <c r="L3" s="14"/>
-      <c r="N3" s="12" t="s">
+      <c r="K3" s="15"/>
+      <c r="L3" s="16"/>
+      <c r="N3" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="O3" s="13"/>
-      <c r="P3" s="14"/>
-      <c r="R3" s="12" t="s">
+      <c r="O3" s="15"/>
+      <c r="P3" s="16"/>
+      <c r="R3" s="14" t="s">
         <v>55</v>
       </c>
-      <c r="S3" s="13"/>
-      <c r="T3" s="14"/>
+      <c r="S3" s="15"/>
+      <c r="T3" s="16"/>
     </row>
     <row r="4" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B4" s="1" t="s">
@@ -1359,11 +1365,11 @@
         <v>2</v>
       </c>
       <c r="D8" s="3"/>
-      <c r="F8" s="12" t="s">
+      <c r="F8" s="14" t="s">
         <v>45</v>
       </c>
-      <c r="G8" s="13"/>
-      <c r="H8" s="14"/>
+      <c r="G8" s="15"/>
+      <c r="H8" s="16"/>
       <c r="J8" s="4" t="s">
         <v>34</v>
       </c>
@@ -1515,11 +1521,11 @@
         <v>1</v>
       </c>
       <c r="P12" s="8"/>
-      <c r="R12" s="12" t="s">
+      <c r="R12" s="14" t="s">
         <v>59</v>
       </c>
-      <c r="S12" s="13"/>
-      <c r="T12" s="14"/>
+      <c r="S12" s="15"/>
+      <c r="T12" s="16"/>
     </row>
     <row r="13" spans="2:20" ht="18" x14ac:dyDescent="0.35">
       <c r="B13" s="4" t="s">
@@ -1529,16 +1535,16 @@
         <v>2</v>
       </c>
       <c r="D13" s="3"/>
-      <c r="F13" s="12" t="s">
+      <c r="F13" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="G13" s="13"/>
-      <c r="H13" s="14"/>
-      <c r="J13" s="12" t="s">
+      <c r="G13" s="15"/>
+      <c r="H13" s="16"/>
+      <c r="J13" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="K13" s="13"/>
-      <c r="L13" s="14"/>
+      <c r="K13" s="15"/>
+      <c r="L13" s="16"/>
       <c r="R13" s="4" t="s">
         <v>11</v>
       </c>
@@ -1573,11 +1579,11 @@
       <c r="L14" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="N14" s="12" t="s">
+      <c r="N14" s="14" t="s">
         <v>73</v>
       </c>
-      <c r="O14" s="13"/>
-      <c r="P14" s="14"/>
+      <c r="O14" s="15"/>
+      <c r="P14" s="16"/>
       <c r="R14" s="4" t="s">
         <v>60</v>
       </c>
@@ -1625,11 +1631,11 @@
       </c>
     </row>
     <row r="16" spans="2:20" ht="18" x14ac:dyDescent="0.35">
-      <c r="B16" s="12" t="s">
+      <c r="B16" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="C16" s="13"/>
-      <c r="D16" s="14"/>
+      <c r="C16" s="15"/>
+      <c r="D16" s="16"/>
       <c r="J16" s="6" t="s">
         <v>37</v>
       </c>
@@ -1664,11 +1670,11 @@
       <c r="D17" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="F17" s="12" t="s">
+      <c r="F17" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="G17" s="13"/>
-      <c r="H17" s="14"/>
+      <c r="G17" s="15"/>
+      <c r="H17" s="16"/>
       <c r="N17" s="6" t="s">
         <v>35</v>
       </c>
@@ -1703,11 +1709,11 @@
         <v>1</v>
       </c>
       <c r="H18" s="3"/>
-      <c r="J18" s="12" t="s">
+      <c r="J18" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="K18" s="13"/>
-      <c r="L18" s="14"/>
+      <c r="K18" s="15"/>
+      <c r="L18" s="16"/>
       <c r="R18" s="4" t="s">
         <v>32</v>
       </c>
@@ -1851,11 +1857,11 @@
         <v>43</v>
       </c>
       <c r="D24" s="8"/>
-      <c r="R24" s="12" t="s">
+      <c r="R24" s="14" t="s">
         <v>66</v>
       </c>
-      <c r="S24" s="13"/>
-      <c r="T24" s="14"/>
+      <c r="S24" s="15"/>
+      <c r="T24" s="16"/>
     </row>
     <row r="25" spans="2:20" x14ac:dyDescent="0.3">
       <c r="R25" s="4" t="s">
@@ -1869,11 +1875,11 @@
       </c>
     </row>
     <row r="26" spans="2:20" ht="18" x14ac:dyDescent="0.35">
-      <c r="B26" s="12" t="s">
+      <c r="B26" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="C26" s="13"/>
-      <c r="D26" s="14"/>
+      <c r="C26" s="15"/>
+      <c r="D26" s="16"/>
       <c r="R26" s="4" t="s">
         <v>60</v>
       </c>
@@ -1941,11 +1947,11 @@
       </c>
     </row>
     <row r="31" spans="2:20" ht="18" x14ac:dyDescent="0.35">
-      <c r="B31" s="12" t="s">
+      <c r="B31" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="C31" s="13"/>
-      <c r="D31" s="14"/>
+      <c r="C31" s="15"/>
+      <c r="D31" s="16"/>
     </row>
     <row r="32" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B32" s="4" t="s">
@@ -1969,6 +1975,11 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="R3:T3"/>
+    <mergeCell ref="R12:T12"/>
+    <mergeCell ref="R24:T24"/>
+    <mergeCell ref="B3:D3"/>
+    <mergeCell ref="B16:D16"/>
     <mergeCell ref="B31:D31"/>
     <mergeCell ref="B26:D26"/>
     <mergeCell ref="N14:P14"/>
@@ -1980,11 +1991,6 @@
     <mergeCell ref="F13:H13"/>
     <mergeCell ref="F17:H17"/>
     <mergeCell ref="N3:P3"/>
-    <mergeCell ref="R3:T3"/>
-    <mergeCell ref="R12:T12"/>
-    <mergeCell ref="R24:T24"/>
-    <mergeCell ref="B3:D3"/>
-    <mergeCell ref="B16:D16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1993,10 +1999,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE0C0E27-F398-4128-B7EC-E6C5B9DA9B0B}">
-  <dimension ref="B2:AE223"/>
+  <dimension ref="B2:AE224"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B198" sqref="B198"/>
+    <sheetView tabSelected="1" topLeftCell="A139" workbookViewId="0">
+      <selection activeCell="D149" sqref="D149"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2009,37 +2015,37 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:6" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="16" t="s">
+      <c r="B2" s="18" t="s">
         <v>79</v>
       </c>
-      <c r="C2" s="17"/>
-      <c r="D2" s="17"/>
-      <c r="E2" s="17"/>
-      <c r="F2" s="18"/>
+      <c r="C2" s="19"/>
+      <c r="D2" s="19"/>
+      <c r="E2" s="19"/>
+      <c r="F2" s="20"/>
     </row>
     <row r="4" spans="2:6" ht="21" x14ac:dyDescent="0.4">
-      <c r="B4" s="15" t="s">
+      <c r="B4" s="17" t="s">
         <v>80</v>
       </c>
-      <c r="C4" s="15"/>
-      <c r="D4" s="15"/>
-      <c r="E4" s="15"/>
-      <c r="F4" s="15"/>
+      <c r="C4" s="17"/>
+      <c r="D4" s="17"/>
+      <c r="E4" s="17"/>
+      <c r="F4" s="17"/>
     </row>
     <row r="6" spans="2:6" ht="18" x14ac:dyDescent="0.35">
-      <c r="B6" s="19" t="s">
+      <c r="B6" s="12" t="s">
         <v>74</v>
       </c>
-      <c r="C6" s="19" t="s">
+      <c r="C6" s="12" t="s">
         <v>75</v>
       </c>
-      <c r="D6" s="20" t="s">
+      <c r="D6" s="13" t="s">
         <v>76</v>
       </c>
-      <c r="E6" s="19" t="s">
+      <c r="E6" s="12" t="s">
         <v>77</v>
       </c>
-      <c r="F6" s="19" t="s">
+      <c r="F6" s="12" t="s">
         <v>78</v>
       </c>
     </row>
@@ -2261,28 +2267,28 @@
       </c>
     </row>
     <row r="21" spans="2:7" ht="21" x14ac:dyDescent="0.4">
-      <c r="B21" s="15" t="s">
+      <c r="B21" s="17" t="s">
         <v>100</v>
       </c>
-      <c r="C21" s="15"/>
-      <c r="D21" s="15"/>
-      <c r="E21" s="15"/>
-      <c r="F21" s="15"/>
+      <c r="C21" s="17"/>
+      <c r="D21" s="17"/>
+      <c r="E21" s="17"/>
+      <c r="F21" s="17"/>
     </row>
     <row r="23" spans="2:7" ht="18" x14ac:dyDescent="0.35">
-      <c r="B23" s="19" t="s">
+      <c r="B23" s="12" t="s">
         <v>74</v>
       </c>
-      <c r="C23" s="19" t="s">
+      <c r="C23" s="12" t="s">
         <v>75</v>
       </c>
-      <c r="D23" s="20" t="s">
+      <c r="D23" s="13" t="s">
         <v>76</v>
       </c>
-      <c r="E23" s="19" t="s">
+      <c r="E23" s="12" t="s">
         <v>77</v>
       </c>
-      <c r="F23" s="19" t="s">
+      <c r="F23" s="12" t="s">
         <v>78</v>
       </c>
     </row>
@@ -2403,28 +2409,28 @@
       </c>
     </row>
     <row r="32" spans="2:7" ht="21" x14ac:dyDescent="0.4">
-      <c r="B32" s="15" t="s">
+      <c r="B32" s="17" t="s">
         <v>93</v>
       </c>
-      <c r="C32" s="15"/>
-      <c r="D32" s="15"/>
-      <c r="E32" s="15"/>
-      <c r="F32" s="15"/>
+      <c r="C32" s="17"/>
+      <c r="D32" s="17"/>
+      <c r="E32" s="17"/>
+      <c r="F32" s="17"/>
     </row>
     <row r="34" spans="2:6" ht="18" x14ac:dyDescent="0.35">
-      <c r="B34" s="19" t="s">
+      <c r="B34" s="12" t="s">
         <v>74</v>
       </c>
-      <c r="C34" s="19" t="s">
+      <c r="C34" s="12" t="s">
         <v>75</v>
       </c>
-      <c r="D34" s="20" t="s">
+      <c r="D34" s="13" t="s">
         <v>76</v>
       </c>
-      <c r="E34" s="19" t="s">
+      <c r="E34" s="12" t="s">
         <v>77</v>
       </c>
-      <c r="F34" s="19" t="s">
+      <c r="F34" s="12" t="s">
         <v>78</v>
       </c>
     </row>
@@ -2595,28 +2601,28 @@
       </c>
     </row>
     <row r="46" spans="2:6" ht="21" x14ac:dyDescent="0.4">
-      <c r="B46" s="15" t="s">
+      <c r="B46" s="17" t="s">
         <v>157</v>
       </c>
-      <c r="C46" s="15"/>
-      <c r="D46" s="15"/>
-      <c r="E46" s="15"/>
-      <c r="F46" s="15"/>
+      <c r="C46" s="17"/>
+      <c r="D46" s="17"/>
+      <c r="E46" s="17"/>
+      <c r="F46" s="17"/>
     </row>
     <row r="48" spans="2:6" ht="18" x14ac:dyDescent="0.35">
-      <c r="B48" s="19" t="s">
+      <c r="B48" s="12" t="s">
         <v>74</v>
       </c>
-      <c r="C48" s="19" t="s">
+      <c r="C48" s="12" t="s">
         <v>75</v>
       </c>
-      <c r="D48" s="20" t="s">
+      <c r="D48" s="13" t="s">
         <v>76</v>
       </c>
-      <c r="E48" s="19" t="s">
+      <c r="E48" s="12" t="s">
         <v>77</v>
       </c>
-      <c r="F48" s="19" t="s">
+      <c r="F48" s="12" t="s">
         <v>78</v>
       </c>
     </row>
@@ -2736,29 +2742,29 @@
       </c>
     </row>
     <row r="57" spans="2:31" ht="21" x14ac:dyDescent="0.4">
-      <c r="B57" s="15" t="s">
+      <c r="B57" s="17" t="s">
         <v>102</v>
       </c>
-      <c r="C57" s="15"/>
-      <c r="D57" s="15"/>
-      <c r="E57" s="15"/>
-      <c r="F57" s="15"/>
+      <c r="C57" s="17"/>
+      <c r="D57" s="17"/>
+      <c r="E57" s="17"/>
+      <c r="F57" s="17"/>
       <c r="AE57" s="10"/>
     </row>
     <row r="59" spans="2:31" ht="18" x14ac:dyDescent="0.35">
-      <c r="B59" s="19" t="s">
+      <c r="B59" s="12" t="s">
         <v>74</v>
       </c>
-      <c r="C59" s="19" t="s">
+      <c r="C59" s="12" t="s">
         <v>75</v>
       </c>
-      <c r="D59" s="20" t="s">
+      <c r="D59" s="13" t="s">
         <v>76</v>
       </c>
-      <c r="E59" s="19" t="s">
+      <c r="E59" s="12" t="s">
         <v>77</v>
       </c>
-      <c r="F59" s="19" t="s">
+      <c r="F59" s="12" t="s">
         <v>78</v>
       </c>
     </row>
@@ -2861,29 +2867,29 @@
       </c>
     </row>
     <row r="67" spans="2:31" ht="21" x14ac:dyDescent="0.4">
-      <c r="B67" s="15" t="s">
+      <c r="B67" s="17" t="s">
         <v>105</v>
       </c>
-      <c r="C67" s="15"/>
-      <c r="D67" s="15"/>
-      <c r="E67" s="15"/>
-      <c r="F67" s="15"/>
+      <c r="C67" s="17"/>
+      <c r="D67" s="17"/>
+      <c r="E67" s="17"/>
+      <c r="F67" s="17"/>
       <c r="AE67" s="10"/>
     </row>
     <row r="69" spans="2:31" ht="18" x14ac:dyDescent="0.35">
-      <c r="B69" s="19" t="s">
+      <c r="B69" s="12" t="s">
         <v>74</v>
       </c>
-      <c r="C69" s="19" t="s">
+      <c r="C69" s="12" t="s">
         <v>75</v>
       </c>
-      <c r="D69" s="20" t="s">
+      <c r="D69" s="13" t="s">
         <v>76</v>
       </c>
-      <c r="E69" s="19" t="s">
+      <c r="E69" s="12" t="s">
         <v>77</v>
       </c>
-      <c r="F69" s="19" t="s">
+      <c r="F69" s="12" t="s">
         <v>78</v>
       </c>
     </row>
@@ -2969,29 +2975,29 @@
       </c>
     </row>
     <row r="76" spans="2:31" ht="21" x14ac:dyDescent="0.4">
-      <c r="B76" s="15" t="s">
+      <c r="B76" s="17" t="s">
         <v>107</v>
       </c>
-      <c r="C76" s="15"/>
-      <c r="D76" s="15"/>
-      <c r="E76" s="15"/>
-      <c r="F76" s="15"/>
+      <c r="C76" s="17"/>
+      <c r="D76" s="17"/>
+      <c r="E76" s="17"/>
+      <c r="F76" s="17"/>
       <c r="AE76" s="10"/>
     </row>
     <row r="78" spans="2:31" ht="18" x14ac:dyDescent="0.35">
-      <c r="B78" s="19" t="s">
+      <c r="B78" s="12" t="s">
         <v>74</v>
       </c>
-      <c r="C78" s="19" t="s">
+      <c r="C78" s="12" t="s">
         <v>75</v>
       </c>
-      <c r="D78" s="20" t="s">
+      <c r="D78" s="13" t="s">
         <v>76</v>
       </c>
-      <c r="E78" s="19" t="s">
+      <c r="E78" s="12" t="s">
         <v>77</v>
       </c>
-      <c r="F78" s="19" t="s">
+      <c r="F78" s="12" t="s">
         <v>78</v>
       </c>
     </row>
@@ -3101,28 +3107,28 @@
     </row>
     <row r="85" spans="2:31" ht="16.2" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="86" spans="2:31" ht="21" x14ac:dyDescent="0.4">
-      <c r="B86" s="15" t="s">
+      <c r="B86" s="17" t="s">
         <v>109</v>
       </c>
-      <c r="C86" s="15"/>
-      <c r="D86" s="15"/>
-      <c r="E86" s="15"/>
-      <c r="F86" s="15"/>
+      <c r="C86" s="17"/>
+      <c r="D86" s="17"/>
+      <c r="E86" s="17"/>
+      <c r="F86" s="17"/>
     </row>
     <row r="88" spans="2:31" ht="18" x14ac:dyDescent="0.35">
-      <c r="B88" s="19" t="s">
+      <c r="B88" s="12" t="s">
         <v>74</v>
       </c>
-      <c r="C88" s="19" t="s">
+      <c r="C88" s="12" t="s">
         <v>75</v>
       </c>
-      <c r="D88" s="20" t="s">
+      <c r="D88" s="13" t="s">
         <v>76</v>
       </c>
-      <c r="E88" s="19" t="s">
+      <c r="E88" s="12" t="s">
         <v>77</v>
       </c>
-      <c r="F88" s="19" t="s">
+      <c r="F88" s="12" t="s">
         <v>78</v>
       </c>
     </row>
@@ -3250,28 +3256,28 @@
       <c r="F96" s="5"/>
     </row>
     <row r="97" spans="2:31" ht="21" x14ac:dyDescent="0.4">
-      <c r="B97" s="15" t="s">
+      <c r="B97" s="17" t="s">
         <v>111</v>
       </c>
-      <c r="C97" s="15"/>
-      <c r="D97" s="15"/>
-      <c r="E97" s="15"/>
-      <c r="F97" s="15"/>
+      <c r="C97" s="17"/>
+      <c r="D97" s="17"/>
+      <c r="E97" s="17"/>
+      <c r="F97" s="17"/>
     </row>
     <row r="99" spans="2:31" ht="18" x14ac:dyDescent="0.35">
-      <c r="B99" s="19" t="s">
+      <c r="B99" s="12" t="s">
         <v>74</v>
       </c>
-      <c r="C99" s="19" t="s">
+      <c r="C99" s="12" t="s">
         <v>75</v>
       </c>
-      <c r="D99" s="20" t="s">
+      <c r="D99" s="13" t="s">
         <v>76</v>
       </c>
-      <c r="E99" s="19" t="s">
+      <c r="E99" s="12" t="s">
         <v>77</v>
       </c>
-      <c r="F99" s="19" t="s">
+      <c r="F99" s="12" t="s">
         <v>78</v>
       </c>
     </row>
@@ -3375,30 +3381,30 @@
       </c>
     </row>
     <row r="107" spans="2:31" ht="21" x14ac:dyDescent="0.4">
-      <c r="B107" s="15" t="s">
+      <c r="B107" s="17" t="s">
         <v>112</v>
       </c>
-      <c r="C107" s="15"/>
-      <c r="D107" s="15"/>
-      <c r="E107" s="15"/>
-      <c r="F107" s="15"/>
+      <c r="C107" s="17"/>
+      <c r="D107" s="17"/>
+      <c r="E107" s="17"/>
+      <c r="F107" s="17"/>
       <c r="AE107" s="10"/>
     </row>
     <row r="108" spans="2:31" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="109" spans="2:31" ht="18" x14ac:dyDescent="0.35">
-      <c r="B109" s="19" t="s">
+      <c r="B109" s="12" t="s">
         <v>74</v>
       </c>
-      <c r="C109" s="19" t="s">
+      <c r="C109" s="12" t="s">
         <v>75</v>
       </c>
-      <c r="D109" s="20" t="s">
+      <c r="D109" s="13" t="s">
         <v>76</v>
       </c>
-      <c r="E109" s="19" t="s">
+      <c r="E109" s="12" t="s">
         <v>77</v>
       </c>
-      <c r="F109" s="19" t="s">
+      <c r="F109" s="12" t="s">
         <v>78</v>
       </c>
     </row>
@@ -3484,28 +3490,28 @@
       </c>
     </row>
     <row r="116" spans="2:31" ht="21" x14ac:dyDescent="0.4">
-      <c r="B116" s="15" t="s">
+      <c r="B116" s="17" t="s">
         <v>114</v>
       </c>
-      <c r="C116" s="15"/>
-      <c r="D116" s="15"/>
-      <c r="E116" s="15"/>
-      <c r="F116" s="15"/>
+      <c r="C116" s="17"/>
+      <c r="D116" s="17"/>
+      <c r="E116" s="17"/>
+      <c r="F116" s="17"/>
     </row>
     <row r="118" spans="2:31" ht="18" x14ac:dyDescent="0.35">
-      <c r="B118" s="19" t="s">
+      <c r="B118" s="12" t="s">
         <v>74</v>
       </c>
-      <c r="C118" s="19" t="s">
+      <c r="C118" s="12" t="s">
         <v>75</v>
       </c>
-      <c r="D118" s="20" t="s">
+      <c r="D118" s="13" t="s">
         <v>76</v>
       </c>
-      <c r="E118" s="19" t="s">
+      <c r="E118" s="12" t="s">
         <v>77</v>
       </c>
-      <c r="F118" s="19" t="s">
+      <c r="F118" s="12" t="s">
         <v>78</v>
       </c>
     </row>
@@ -3552,7 +3558,7 @@
         <v>2</v>
       </c>
       <c r="D121" s="11">
-        <v>100</v>
+        <v>150</v>
       </c>
       <c r="E121" s="5" t="s">
         <v>81</v>
@@ -3563,7 +3569,7 @@
     </row>
     <row r="122" spans="2:31" x14ac:dyDescent="0.3">
       <c r="B122" s="5" t="s">
-        <v>31</v>
+        <v>182</v>
       </c>
       <c r="C122" s="5" t="s">
         <v>1</v>
@@ -3665,23 +3671,24 @@
     </row>
     <row r="128" spans="2:31" x14ac:dyDescent="0.3">
       <c r="B128" s="9" t="s">
+        <v>183</v>
+      </c>
+      <c r="C128" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="D128" s="11">
+        <v>11</v>
+      </c>
+      <c r="E128" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="F128" s="9" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="129" spans="2:31" x14ac:dyDescent="0.3">
+      <c r="B129" s="9" t="s">
         <v>131</v>
-      </c>
-      <c r="C128" s="9" t="s">
-        <v>91</v>
-      </c>
-      <c r="D128" s="11"/>
-      <c r="E128" s="9" t="s">
-        <v>82</v>
-      </c>
-      <c r="F128" s="9" t="s">
-        <v>136</v>
-      </c>
-      <c r="AE128" s="10"/>
-    </row>
-    <row r="129" spans="2:31" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B129" s="9" t="s">
-        <v>129</v>
       </c>
       <c r="C129" s="9" t="s">
         <v>91</v>
@@ -3691,72 +3698,71 @@
         <v>82</v>
       </c>
       <c r="F129" s="9" t="s">
-        <v>137</v>
-      </c>
+        <v>136</v>
+      </c>
+      <c r="AE129" s="10"/>
     </row>
     <row r="130" spans="2:31" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B130" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="C130" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="D130" s="11"/>
+      <c r="E130" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="F130" s="9" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="131" spans="2:31" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B131" s="9" t="s">
         <v>83</v>
       </c>
-      <c r="C130" s="9" t="s">
+      <c r="C131" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="D130" s="11">
-        <v>2</v>
-      </c>
-      <c r="E130" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="F130" s="5" t="s">
+      <c r="D131" s="11">
+        <v>2</v>
+      </c>
+      <c r="E131" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="F131" s="5" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="132" spans="2:31" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B132" s="15" t="s">
+    <row r="133" spans="2:31" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B133" s="17" t="s">
         <v>117</v>
       </c>
-      <c r="C132" s="15"/>
-      <c r="D132" s="15"/>
-      <c r="E132" s="15"/>
-      <c r="F132" s="15"/>
-    </row>
-    <row r="134" spans="2:31" ht="18" x14ac:dyDescent="0.35">
-      <c r="B134" s="19" t="s">
+      <c r="C133" s="17"/>
+      <c r="D133" s="17"/>
+      <c r="E133" s="17"/>
+      <c r="F133" s="17"/>
+    </row>
+    <row r="135" spans="2:31" ht="18" x14ac:dyDescent="0.35">
+      <c r="B135" s="12" t="s">
         <v>74</v>
       </c>
-      <c r="C134" s="19" t="s">
+      <c r="C135" s="12" t="s">
         <v>75</v>
       </c>
-      <c r="D134" s="20" t="s">
+      <c r="D135" s="13" t="s">
         <v>76</v>
       </c>
-      <c r="E134" s="19" t="s">
+      <c r="E135" s="12" t="s">
         <v>77</v>
       </c>
-      <c r="F134" s="19" t="s">
+      <c r="F135" s="12" t="s">
         <v>78</v>
-      </c>
-    </row>
-    <row r="135" spans="2:31" x14ac:dyDescent="0.3">
-      <c r="B135" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C135" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="D135" s="11">
-        <v>11</v>
-      </c>
-      <c r="E135" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="F135" s="5" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="136" spans="2:31" x14ac:dyDescent="0.3">
       <c r="B136" s="5" t="s">
-        <v>35</v>
+        <v>11</v>
       </c>
       <c r="C136" s="5" t="s">
         <v>1</v>
@@ -3768,45 +3774,46 @@
         <v>81</v>
       </c>
       <c r="F136" s="5" t="s">
-        <v>116</v>
+        <v>84</v>
       </c>
     </row>
     <row r="137" spans="2:31" x14ac:dyDescent="0.3">
       <c r="B137" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="C137" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="D137" s="11">
+        <v>11</v>
+      </c>
+      <c r="E137" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="F137" s="5" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="138" spans="2:31" x14ac:dyDescent="0.3">
+      <c r="B138" s="5" t="s">
         <v>176</v>
       </c>
-      <c r="C137" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="D137" s="11">
-        <v>100</v>
-      </c>
-      <c r="E137" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="F137" s="5" t="s">
+      <c r="C138" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D138" s="11">
+        <v>150</v>
+      </c>
+      <c r="E138" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="F138" s="5" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="138" spans="2:31" x14ac:dyDescent="0.3">
-      <c r="B138" s="9" t="s">
+    <row r="139" spans="2:31" x14ac:dyDescent="0.3">
+      <c r="B139" s="9" t="s">
         <v>131</v>
-      </c>
-      <c r="C138" s="9" t="s">
-        <v>91</v>
-      </c>
-      <c r="D138" s="11"/>
-      <c r="E138" s="9" t="s">
-        <v>82</v>
-      </c>
-      <c r="F138" s="9" t="s">
-        <v>138</v>
-      </c>
-      <c r="AE138" s="10"/>
-    </row>
-    <row r="139" spans="2:31" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B139" s="9" t="s">
-        <v>129</v>
       </c>
       <c r="C139" s="9" t="s">
         <v>91</v>
@@ -3816,72 +3823,71 @@
         <v>82</v>
       </c>
       <c r="F139" s="9" t="s">
-        <v>139</v>
-      </c>
+        <v>138</v>
+      </c>
+      <c r="AE139" s="10"/>
     </row>
     <row r="140" spans="2:31" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B140" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="C140" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="D140" s="11"/>
+      <c r="E140" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="F140" s="9" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="141" spans="2:31" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B141" s="9" t="s">
         <v>83</v>
       </c>
-      <c r="C140" s="9" t="s">
+      <c r="C141" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="D140" s="11">
-        <v>2</v>
-      </c>
-      <c r="E140" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="F140" s="5" t="s">
+      <c r="D141" s="11">
+        <v>2</v>
+      </c>
+      <c r="E141" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="F141" s="5" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="142" spans="2:31" ht="21" x14ac:dyDescent="0.4">
-      <c r="B142" s="15" t="s">
+    <row r="143" spans="2:31" ht="21" x14ac:dyDescent="0.4">
+      <c r="B143" s="17" t="s">
         <v>118</v>
       </c>
-      <c r="C142" s="15"/>
-      <c r="D142" s="15"/>
-      <c r="E142" s="15"/>
-      <c r="F142" s="15"/>
-    </row>
-    <row r="144" spans="2:31" ht="18" x14ac:dyDescent="0.35">
-      <c r="B144" s="19" t="s">
+      <c r="C143" s="17"/>
+      <c r="D143" s="17"/>
+      <c r="E143" s="17"/>
+      <c r="F143" s="17"/>
+    </row>
+    <row r="145" spans="2:31" ht="18" x14ac:dyDescent="0.35">
+      <c r="B145" s="12" t="s">
         <v>74</v>
       </c>
-      <c r="C144" s="19" t="s">
+      <c r="C145" s="12" t="s">
         <v>75</v>
       </c>
-      <c r="D144" s="20" t="s">
+      <c r="D145" s="13" t="s">
         <v>76</v>
       </c>
-      <c r="E144" s="19" t="s">
+      <c r="E145" s="12" t="s">
         <v>77</v>
       </c>
-      <c r="F144" s="19" t="s">
+      <c r="F145" s="12" t="s">
         <v>78</v>
-      </c>
-    </row>
-    <row r="145" spans="2:31" x14ac:dyDescent="0.3">
-      <c r="B145" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C145" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="D145" s="11">
-        <v>11</v>
-      </c>
-      <c r="E145" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="F145" s="5" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="146" spans="2:31" x14ac:dyDescent="0.3">
       <c r="B146" s="5" t="s">
-        <v>35</v>
+        <v>11</v>
       </c>
       <c r="C146" s="5" t="s">
         <v>1</v>
@@ -3893,12 +3899,12 @@
         <v>81</v>
       </c>
       <c r="F146" s="5" t="s">
-        <v>116</v>
+        <v>84</v>
       </c>
     </row>
     <row r="147" spans="2:31" x14ac:dyDescent="0.3">
       <c r="B147" s="5" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="C147" s="5" t="s">
         <v>1</v>
@@ -3910,44 +3916,46 @@
         <v>81</v>
       </c>
       <c r="F147" s="5" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
     </row>
     <row r="148" spans="2:31" x14ac:dyDescent="0.3">
       <c r="B148" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C148" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="D148" s="11">
+        <v>11</v>
+      </c>
+      <c r="E148" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="F148" s="5" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="149" spans="2:31" x14ac:dyDescent="0.3">
+      <c r="B149" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="C148" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="D148" s="11">
-        <v>100</v>
-      </c>
-      <c r="E148" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="F148" s="5" t="s">
+      <c r="C149" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D149" s="11">
+        <v>150</v>
+      </c>
+      <c r="E149" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="F149" s="5" t="s">
         <v>115</v>
-      </c>
-    </row>
-    <row r="149" spans="2:31" x14ac:dyDescent="0.3">
-      <c r="B149" s="9" t="s">
-        <v>131</v>
-      </c>
-      <c r="C149" s="9" t="s">
-        <v>91</v>
-      </c>
-      <c r="D149" s="11"/>
-      <c r="E149" s="9" t="s">
-        <v>82</v>
-      </c>
-      <c r="F149" s="9" t="s">
-        <v>140</v>
       </c>
     </row>
     <row r="150" spans="2:31" x14ac:dyDescent="0.3">
       <c r="B150" s="9" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="C150" s="9" t="s">
         <v>91</v>
@@ -3957,94 +3965,92 @@
         <v>82</v>
       </c>
       <c r="F150" s="9" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="151" spans="2:31" x14ac:dyDescent="0.3">
       <c r="B151" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="C151" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="D151" s="11"/>
+      <c r="E151" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="F151" s="9" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="152" spans="2:31" x14ac:dyDescent="0.3">
+      <c r="B152" s="9" t="s">
         <v>83</v>
       </c>
-      <c r="C151" s="9" t="s">
+      <c r="C152" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="D151" s="11">
-        <v>2</v>
-      </c>
-      <c r="E151" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="F151" s="5" t="s">
+      <c r="D152" s="11">
+        <v>2</v>
+      </c>
+      <c r="E152" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="F152" s="5" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="153" spans="2:31" ht="21" x14ac:dyDescent="0.4">
-      <c r="B153" s="15" t="s">
+    <row r="154" spans="2:31" ht="21" x14ac:dyDescent="0.4">
+      <c r="B154" s="17" t="s">
         <v>120</v>
       </c>
-      <c r="C153" s="15"/>
-      <c r="D153" s="15"/>
-      <c r="E153" s="15"/>
-      <c r="F153" s="15"/>
-    </row>
-    <row r="154" spans="2:31" x14ac:dyDescent="0.3">
-      <c r="AE154" s="10"/>
-    </row>
-    <row r="155" spans="2:31" ht="18" x14ac:dyDescent="0.35">
-      <c r="B155" s="19" t="s">
+      <c r="C154" s="17"/>
+      <c r="D154" s="17"/>
+      <c r="E154" s="17"/>
+      <c r="F154" s="17"/>
+    </row>
+    <row r="155" spans="2:31" x14ac:dyDescent="0.3">
+      <c r="AE155" s="10"/>
+    </row>
+    <row r="156" spans="2:31" ht="18" x14ac:dyDescent="0.35">
+      <c r="B156" s="12" t="s">
         <v>74</v>
       </c>
-      <c r="C155" s="19" t="s">
+      <c r="C156" s="12" t="s">
         <v>75</v>
       </c>
-      <c r="D155" s="20" t="s">
+      <c r="D156" s="13" t="s">
         <v>76</v>
       </c>
-      <c r="E155" s="19" t="s">
+      <c r="E156" s="12" t="s">
         <v>77</v>
       </c>
-      <c r="F155" s="19" t="s">
+      <c r="F156" s="12" t="s">
         <v>78</v>
-      </c>
-    </row>
-    <row r="156" spans="2:31" x14ac:dyDescent="0.3">
-      <c r="B156" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C156" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="D156" s="11">
-        <v>11</v>
-      </c>
-      <c r="E156" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="F156" s="5" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="157" spans="2:31" x14ac:dyDescent="0.3">
       <c r="B157" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C157" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="D157" s="11">
+        <v>11</v>
+      </c>
+      <c r="E157" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="F157" s="5" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="158" spans="2:31" x14ac:dyDescent="0.3">
+      <c r="B158" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="C157" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="D157" s="11">
-        <v>11</v>
-      </c>
-      <c r="E157" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="F157" s="5" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="158" spans="2:31" x14ac:dyDescent="0.3">
-      <c r="B158" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="C158" s="9" t="s">
+      <c r="C158" s="5" t="s">
         <v>1</v>
       </c>
       <c r="D158" s="11">
@@ -4058,42 +4064,42 @@
       </c>
     </row>
     <row r="159" spans="2:31" x14ac:dyDescent="0.3">
-      <c r="B159" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="C159" s="5" t="s">
-        <v>2</v>
+      <c r="B159" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="C159" s="9" t="s">
+        <v>1</v>
       </c>
       <c r="D159" s="11">
-        <v>100</v>
+        <v>11</v>
       </c>
       <c r="E159" s="5" t="s">
         <v>81</v>
       </c>
       <c r="F159" s="5" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
     </row>
     <row r="160" spans="2:31" x14ac:dyDescent="0.3">
       <c r="B160" s="5" t="s">
-        <v>69</v>
+        <v>51</v>
       </c>
       <c r="C160" s="5" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D160" s="11">
-        <v>11</v>
+        <v>100</v>
       </c>
       <c r="E160" s="5" t="s">
         <v>81</v>
       </c>
       <c r="F160" s="5" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="161" spans="2:31" x14ac:dyDescent="0.3">
       <c r="B161" s="5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C161" s="5" t="s">
         <v>1</v>
@@ -4107,46 +4113,46 @@
       <c r="F161" s="5" t="s">
         <v>116</v>
       </c>
-      <c r="AE161" s="10"/>
     </row>
     <row r="162" spans="2:31" x14ac:dyDescent="0.3">
-      <c r="B162" s="9" t="s">
+      <c r="B162" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="C162" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="D162" s="11">
+        <v>11</v>
+      </c>
+      <c r="E162" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="F162" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="AE162" s="10"/>
+    </row>
+    <row r="163" spans="2:31" x14ac:dyDescent="0.3">
+      <c r="B163" s="9" t="s">
         <v>177</v>
       </c>
-      <c r="C162" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="D162" s="11">
-        <v>11</v>
-      </c>
-      <c r="E162" s="9" t="s">
-        <v>81</v>
-      </c>
-      <c r="F162" s="9" t="s">
+      <c r="C163" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="D163" s="11">
+        <v>11</v>
+      </c>
+      <c r="E163" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="F163" s="9" t="s">
         <v>116</v>
       </c>
-      <c r="AE162" s="10"/>
-    </row>
-    <row r="163" spans="2:31" x14ac:dyDescent="0.3">
-      <c r="B163" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="C163" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="D163" s="11">
-        <v>11</v>
-      </c>
-      <c r="E163" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="F163" s="5" t="s">
-        <v>115</v>
-      </c>
+      <c r="AE163" s="10"/>
     </row>
     <row r="164" spans="2:31" x14ac:dyDescent="0.3">
       <c r="B164" s="5" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C164" s="5" t="s">
         <v>1</v>
@@ -4163,7 +4169,7 @@
     </row>
     <row r="165" spans="2:31" x14ac:dyDescent="0.3">
       <c r="B165" s="5" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C165" s="5" t="s">
         <v>1</v>
@@ -4179,23 +4185,25 @@
       </c>
     </row>
     <row r="166" spans="2:31" x14ac:dyDescent="0.3">
-      <c r="B166" s="9" t="s">
-        <v>131</v>
-      </c>
-      <c r="C166" s="9" t="s">
-        <v>91</v>
-      </c>
-      <c r="D166" s="11"/>
-      <c r="E166" s="9" t="s">
-        <v>82</v>
-      </c>
-      <c r="F166" s="9" t="s">
-        <v>142</v>
+      <c r="B166" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="C166" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="D166" s="11">
+        <v>11</v>
+      </c>
+      <c r="E166" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="F166" s="5" t="s">
+        <v>115</v>
       </c>
     </row>
     <row r="167" spans="2:31" x14ac:dyDescent="0.3">
       <c r="B167" s="9" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="C167" s="9" t="s">
         <v>91</v>
@@ -4205,92 +4213,89 @@
         <v>82</v>
       </c>
       <c r="F167" s="9" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="168" spans="2:31" x14ac:dyDescent="0.3">
       <c r="B168" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="C168" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="D168" s="11"/>
+      <c r="E168" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="F168" s="9" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="169" spans="2:31" x14ac:dyDescent="0.3">
+      <c r="B169" s="9" t="s">
         <v>83</v>
       </c>
-      <c r="C168" s="9" t="s">
+      <c r="C169" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="D168" s="11">
-        <v>2</v>
-      </c>
-      <c r="E168" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="F168" s="5" t="s">
+      <c r="D169" s="11">
+        <v>2</v>
+      </c>
+      <c r="E169" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="F169" s="5" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="170" spans="2:31" ht="21" x14ac:dyDescent="0.4">
-      <c r="B170" s="15" t="s">
+    <row r="171" spans="2:31" ht="21" x14ac:dyDescent="0.4">
+      <c r="B171" s="17" t="s">
         <v>121</v>
       </c>
-      <c r="C170" s="15"/>
-      <c r="D170" s="15"/>
-      <c r="E170" s="15"/>
-      <c r="F170" s="15"/>
-    </row>
-    <row r="172" spans="2:31" ht="18" x14ac:dyDescent="0.35">
-      <c r="B172" s="19" t="s">
+      <c r="C171" s="17"/>
+      <c r="D171" s="17"/>
+      <c r="E171" s="17"/>
+      <c r="F171" s="17"/>
+    </row>
+    <row r="173" spans="2:31" ht="18" x14ac:dyDescent="0.35">
+      <c r="B173" s="12" t="s">
         <v>74</v>
       </c>
-      <c r="C172" s="19" t="s">
+      <c r="C173" s="12" t="s">
         <v>75</v>
       </c>
-      <c r="D172" s="20" t="s">
+      <c r="D173" s="13" t="s">
         <v>76</v>
       </c>
-      <c r="E172" s="19" t="s">
+      <c r="E173" s="12" t="s">
         <v>77</v>
       </c>
-      <c r="F172" s="19" t="s">
+      <c r="F173" s="12" t="s">
         <v>78</v>
-      </c>
-    </row>
-    <row r="173" spans="2:31" x14ac:dyDescent="0.3">
-      <c r="B173" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C173" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="D173" s="11">
-        <v>11</v>
-      </c>
-      <c r="E173" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="F173" s="5" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="174" spans="2:31" x14ac:dyDescent="0.3">
       <c r="B174" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C174" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="D174" s="11">
+        <v>11</v>
+      </c>
+      <c r="E174" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="F174" s="5" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="175" spans="2:31" x14ac:dyDescent="0.3">
+      <c r="B175" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="C174" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="D174" s="11">
-        <v>11</v>
-      </c>
-      <c r="E174" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="F174" s="5" t="s">
-        <v>116</v>
-      </c>
-      <c r="AE174" s="10"/>
-    </row>
-    <row r="175" spans="2:31" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B175" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="C175" s="9" t="s">
+      <c r="C175" s="5" t="s">
         <v>1</v>
       </c>
       <c r="D175" s="11">
@@ -4302,25 +4307,28 @@
       <c r="F175" s="5" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="176" spans="2:31" x14ac:dyDescent="0.3">
+      <c r="AE175" s="10"/>
+    </row>
+    <row r="176" spans="2:31" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B176" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="C176" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="D176" s="11">
+        <v>11</v>
+      </c>
+      <c r="E176" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="F176" s="5" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="177" spans="2:31" x14ac:dyDescent="0.3">
+      <c r="B177" s="9" t="s">
         <v>131</v>
-      </c>
-      <c r="C176" s="9" t="s">
-        <v>91</v>
-      </c>
-      <c r="D176" s="11"/>
-      <c r="E176" s="9" t="s">
-        <v>82</v>
-      </c>
-      <c r="F176" s="9" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="177" spans="2:31" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B177" s="9" t="s">
-        <v>129</v>
       </c>
       <c r="C177" s="9" t="s">
         <v>91</v>
@@ -4330,72 +4338,70 @@
         <v>82</v>
       </c>
       <c r="F177" s="9" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="178" spans="2:31" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B178" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="C178" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="D178" s="11"/>
+      <c r="E178" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="F178" s="9" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="179" spans="2:31" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B179" s="9" t="s">
         <v>83</v>
       </c>
-      <c r="C178" s="9" t="s">
+      <c r="C179" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="D178" s="11">
-        <v>2</v>
-      </c>
-      <c r="E178" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="F178" s="5" t="s">
+      <c r="D179" s="11">
+        <v>2</v>
+      </c>
+      <c r="E179" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="F179" s="5" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="180" spans="2:31" ht="21" x14ac:dyDescent="0.4">
-      <c r="B180" s="15" t="s">
+    <row r="181" spans="2:31" ht="21" x14ac:dyDescent="0.4">
+      <c r="B181" s="17" t="s">
         <v>122</v>
       </c>
-      <c r="C180" s="15"/>
-      <c r="D180" s="15"/>
-      <c r="E180" s="15"/>
-      <c r="F180" s="15"/>
-    </row>
-    <row r="182" spans="2:31" ht="18" x14ac:dyDescent="0.35">
-      <c r="B182" s="19" t="s">
+      <c r="C181" s="17"/>
+      <c r="D181" s="17"/>
+      <c r="E181" s="17"/>
+      <c r="F181" s="17"/>
+    </row>
+    <row r="183" spans="2:31" ht="18" x14ac:dyDescent="0.35">
+      <c r="B183" s="12" t="s">
         <v>74</v>
       </c>
-      <c r="C182" s="19" t="s">
+      <c r="C183" s="12" t="s">
         <v>75</v>
       </c>
-      <c r="D182" s="20" t="s">
+      <c r="D183" s="13" t="s">
         <v>76</v>
       </c>
-      <c r="E182" s="19" t="s">
+      <c r="E183" s="12" t="s">
         <v>77</v>
       </c>
-      <c r="F182" s="19" t="s">
+      <c r="F183" s="12" t="s">
         <v>78</v>
-      </c>
-    </row>
-    <row r="183" spans="2:31" x14ac:dyDescent="0.3">
-      <c r="B183" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C183" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="D183" s="11">
-        <v>11</v>
-      </c>
-      <c r="E183" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="F183" s="5" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="184" spans="2:31" x14ac:dyDescent="0.3">
       <c r="B184" s="5" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="C184" s="5" t="s">
         <v>1</v>
@@ -4407,44 +4413,44 @@
         <v>81</v>
       </c>
       <c r="F184" s="5" t="s">
-        <v>116</v>
+        <v>84</v>
       </c>
     </row>
     <row r="185" spans="2:31" x14ac:dyDescent="0.3">
       <c r="B185" s="5" t="s">
-        <v>56</v>
+        <v>18</v>
       </c>
       <c r="C185" s="5" t="s">
-        <v>91</v>
-      </c>
-      <c r="D185" s="11"/>
+        <v>1</v>
+      </c>
+      <c r="D185" s="11">
+        <v>11</v>
+      </c>
       <c r="E185" s="5" t="s">
         <v>81</v>
       </c>
       <c r="F185" s="5" t="s">
-        <v>123</v>
+        <v>116</v>
       </c>
     </row>
     <row r="186" spans="2:31" x14ac:dyDescent="0.3">
       <c r="B186" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C186" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="D186" s="11">
-        <v>11</v>
-      </c>
+        <v>91</v>
+      </c>
+      <c r="D186" s="11"/>
       <c r="E186" s="5" t="s">
         <v>81</v>
       </c>
       <c r="F186" s="5" t="s">
-        <v>115</v>
+        <v>123</v>
       </c>
     </row>
     <row r="187" spans="2:31" x14ac:dyDescent="0.3">
       <c r="B187" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C187" s="5" t="s">
         <v>1</v>
@@ -4461,14 +4467,16 @@
     </row>
     <row r="188" spans="2:31" x14ac:dyDescent="0.3">
       <c r="B188" s="5" t="s">
-        <v>67</v>
+        <v>58</v>
       </c>
       <c r="C188" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="D188" s="11"/>
+        <v>1</v>
+      </c>
+      <c r="D188" s="11">
+        <v>11</v>
+      </c>
       <c r="E188" s="5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F188" s="5" t="s">
         <v>115</v>
@@ -4476,100 +4484,98 @@
     </row>
     <row r="189" spans="2:31" x14ac:dyDescent="0.3">
       <c r="B189" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="C189" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="D189" s="11"/>
+      <c r="E189" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="F189" s="5" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="190" spans="2:31" x14ac:dyDescent="0.3">
+      <c r="B190" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="C189" s="5" t="s">
+      <c r="C190" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="D189" s="11">
-        <v>11</v>
-      </c>
-      <c r="E189" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="F189" s="5" t="s">
+      <c r="D190" s="11">
+        <v>11</v>
+      </c>
+      <c r="E190" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="F190" s="5" t="s">
         <v>124</v>
       </c>
-      <c r="AE189" s="10"/>
-    </row>
-    <row r="190" spans="2:31" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B190" s="9" t="s">
-        <v>129</v>
-      </c>
-      <c r="C190" s="9" t="s">
-        <v>91</v>
-      </c>
-      <c r="D190" s="11"/>
-      <c r="E190" s="9" t="s">
-        <v>82</v>
-      </c>
-      <c r="F190" s="9" t="s">
-        <v>146</v>
-      </c>
+      <c r="AE190" s="10"/>
     </row>
     <row r="191" spans="2:31" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B191" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="C191" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="D191" s="11"/>
+      <c r="E191" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="F191" s="9" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="192" spans="2:31" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B192" s="9" t="s">
         <v>83</v>
       </c>
-      <c r="C191" s="9" t="s">
+      <c r="C192" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="D191" s="11">
-        <v>2</v>
-      </c>
-      <c r="E191" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="F191" s="5" t="s">
+      <c r="D192" s="11">
+        <v>2</v>
+      </c>
+      <c r="E192" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="F192" s="5" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="193" spans="2:6" ht="21" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B193" s="15" t="s">
+    <row r="194" spans="2:6" ht="21" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B194" s="17" t="s">
         <v>125</v>
       </c>
-      <c r="C193" s="15"/>
-      <c r="D193" s="15"/>
-      <c r="E193" s="15"/>
-      <c r="F193" s="15"/>
-    </row>
-    <row r="195" spans="2:6" ht="18" x14ac:dyDescent="0.35">
-      <c r="B195" s="19" t="s">
+      <c r="C194" s="17"/>
+      <c r="D194" s="17"/>
+      <c r="E194" s="17"/>
+      <c r="F194" s="17"/>
+    </row>
+    <row r="196" spans="2:6" ht="18" x14ac:dyDescent="0.35">
+      <c r="B196" s="12" t="s">
         <v>74</v>
       </c>
-      <c r="C195" s="19" t="s">
+      <c r="C196" s="12" t="s">
         <v>75</v>
       </c>
-      <c r="D195" s="20" t="s">
+      <c r="D196" s="13" t="s">
         <v>76</v>
       </c>
-      <c r="E195" s="19" t="s">
+      <c r="E196" s="12" t="s">
         <v>77</v>
       </c>
-      <c r="F195" s="19" t="s">
+      <c r="F196" s="12" t="s">
         <v>78</v>
-      </c>
-    </row>
-    <row r="196" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B196" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C196" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="D196" s="11">
-        <v>11</v>
-      </c>
-      <c r="E196" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="F196" s="5" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="197" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B197" s="5" t="s">
-        <v>60</v>
+        <v>11</v>
       </c>
       <c r="C197" s="5" t="s">
         <v>1</v>
@@ -4581,12 +4587,12 @@
         <v>81</v>
       </c>
       <c r="F197" s="5" t="s">
-        <v>116</v>
+        <v>84</v>
       </c>
     </row>
     <row r="198" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B198" s="5" t="s">
-        <v>35</v>
+        <v>60</v>
       </c>
       <c r="C198" s="5" t="s">
         <v>1</v>
@@ -4603,24 +4609,24 @@
     </row>
     <row r="199" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B199" s="5" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="C199" s="5" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D199" s="11">
-        <v>50</v>
+        <v>11</v>
       </c>
       <c r="E199" s="5" t="s">
         <v>81</v>
       </c>
       <c r="F199" s="5" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
     </row>
     <row r="200" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B200" s="5" t="s">
-        <v>61</v>
+        <v>29</v>
       </c>
       <c r="C200" s="5" t="s">
         <v>2</v>
@@ -4637,13 +4643,13 @@
     </row>
     <row r="201" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B201" s="5" t="s">
-        <v>181</v>
+        <v>61</v>
       </c>
       <c r="C201" s="5" t="s">
         <v>2</v>
       </c>
       <c r="D201" s="11">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="E201" s="5" t="s">
         <v>81</v>
@@ -4654,13 +4660,13 @@
     </row>
     <row r="202" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B202" s="5" t="s">
-        <v>178</v>
+        <v>181</v>
       </c>
       <c r="C202" s="5" t="s">
         <v>2</v>
       </c>
       <c r="D202" s="11">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="E202" s="5" t="s">
         <v>81</v>
@@ -4670,25 +4676,25 @@
       </c>
     </row>
     <row r="203" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B203" s="9" t="s">
-        <v>179</v>
-      </c>
-      <c r="C203" s="9" t="s">
+      <c r="B203" s="5" t="s">
+        <v>178</v>
+      </c>
+      <c r="C203" s="5" t="s">
         <v>2</v>
       </c>
       <c r="D203" s="11">
         <v>50</v>
       </c>
-      <c r="E203" s="9" t="s">
-        <v>81</v>
-      </c>
-      <c r="F203" s="9" t="s">
+      <c r="E203" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="F203" s="5" t="s">
         <v>115</v>
       </c>
     </row>
     <row r="204" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B204" s="5" t="s">
-        <v>180</v>
+      <c r="B204" s="9" t="s">
+        <v>179</v>
       </c>
       <c r="C204" s="9" t="s">
         <v>2</v>
@@ -4696,22 +4702,22 @@
       <c r="D204" s="11">
         <v>50</v>
       </c>
-      <c r="E204" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="F204" s="5" t="s">
+      <c r="E204" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="F204" s="9" t="s">
         <v>115</v>
       </c>
     </row>
     <row r="205" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B205" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="C205" s="5" t="s">
-        <v>1</v>
+        <v>180</v>
+      </c>
+      <c r="C205" s="9" t="s">
+        <v>2</v>
       </c>
       <c r="D205" s="11">
-        <v>11</v>
+        <v>50</v>
       </c>
       <c r="E205" s="5" t="s">
         <v>81</v>
@@ -4722,7 +4728,7 @@
     </row>
     <row r="206" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B206" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C206" s="5" t="s">
         <v>1</v>
@@ -4739,7 +4745,7 @@
     </row>
     <row r="207" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B207" s="5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C207" s="5" t="s">
         <v>1</v>
@@ -4755,23 +4761,25 @@
       </c>
     </row>
     <row r="208" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B208" s="9" t="s">
-        <v>131</v>
-      </c>
-      <c r="C208" s="9" t="s">
-        <v>91</v>
-      </c>
-      <c r="D208" s="11"/>
-      <c r="E208" s="9" t="s">
-        <v>82</v>
-      </c>
-      <c r="F208" s="9" t="s">
-        <v>148</v>
+      <c r="B208" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="C208" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="D208" s="11">
+        <v>11</v>
+      </c>
+      <c r="E208" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="F208" s="5" t="s">
+        <v>115</v>
       </c>
     </row>
     <row r="209" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B209" s="9" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="C209" s="9" t="s">
         <v>91</v>
@@ -4781,72 +4789,70 @@
         <v>82</v>
       </c>
       <c r="F209" s="9" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
     </row>
     <row r="210" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B210" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="C210" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="D210" s="11"/>
+      <c r="E210" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="F210" s="9" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="211" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B211" s="9" t="s">
         <v>83</v>
       </c>
-      <c r="C210" s="9" t="s">
+      <c r="C211" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="D210" s="11">
-        <v>2</v>
-      </c>
-      <c r="E210" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="F210" s="5" t="s">
+      <c r="D211" s="11">
+        <v>2</v>
+      </c>
+      <c r="E211" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="F211" s="5" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="212" spans="2:6" ht="21" x14ac:dyDescent="0.4">
-      <c r="B212" s="15" t="s">
+    <row r="213" spans="2:6" ht="21" x14ac:dyDescent="0.4">
+      <c r="B213" s="17" t="s">
         <v>126</v>
       </c>
-      <c r="C212" s="15"/>
-      <c r="D212" s="15"/>
-      <c r="E212" s="15"/>
-      <c r="F212" s="15"/>
-    </row>
-    <row r="214" spans="2:6" ht="18" x14ac:dyDescent="0.35">
-      <c r="B214" s="19" t="s">
+      <c r="C213" s="17"/>
+      <c r="D213" s="17"/>
+      <c r="E213" s="17"/>
+      <c r="F213" s="17"/>
+    </row>
+    <row r="215" spans="2:6" ht="18" x14ac:dyDescent="0.35">
+      <c r="B215" s="12" t="s">
         <v>74</v>
       </c>
-      <c r="C214" s="19" t="s">
+      <c r="C215" s="12" t="s">
         <v>75</v>
       </c>
-      <c r="D214" s="20" t="s">
+      <c r="D215" s="13" t="s">
         <v>76</v>
       </c>
-      <c r="E214" s="19" t="s">
+      <c r="E215" s="12" t="s">
         <v>77</v>
       </c>
-      <c r="F214" s="19" t="s">
+      <c r="F215" s="12" t="s">
         <v>78</v>
-      </c>
-    </row>
-    <row r="215" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B215" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C215" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="D215" s="11">
-        <v>11</v>
-      </c>
-      <c r="E215" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="F215" s="5" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="216" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B216" s="5" t="s">
-        <v>60</v>
+        <v>11</v>
       </c>
       <c r="C216" s="5" t="s">
         <v>1</v>
@@ -4858,46 +4864,46 @@
         <v>81</v>
       </c>
       <c r="F216" s="5" t="s">
-        <v>116</v>
+        <v>84</v>
       </c>
     </row>
     <row r="217" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B217" s="5" t="s">
-        <v>20</v>
+        <v>60</v>
       </c>
       <c r="C217" s="5" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D217" s="11">
-        <v>50</v>
+        <v>11</v>
       </c>
       <c r="E217" s="5" t="s">
         <v>81</v>
       </c>
       <c r="F217" s="5" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
     </row>
     <row r="218" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B218" s="5" t="s">
-        <v>154</v>
+        <v>20</v>
       </c>
       <c r="C218" s="5" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D218" s="11">
-        <v>11</v>
+        <v>50</v>
       </c>
       <c r="E218" s="5" t="s">
         <v>81</v>
       </c>
       <c r="F218" s="5" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="219" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B219" s="5" t="s">
-        <v>22</v>
+        <v>154</v>
       </c>
       <c r="C219" s="5" t="s">
         <v>1</v>
@@ -4914,7 +4920,7 @@
     </row>
     <row r="220" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B220" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C220" s="5" t="s">
         <v>1</v>
@@ -4930,23 +4936,25 @@
       </c>
     </row>
     <row r="221" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B221" s="9" t="s">
-        <v>131</v>
-      </c>
-      <c r="C221" s="9" t="s">
-        <v>91</v>
-      </c>
-      <c r="D221" s="11"/>
-      <c r="E221" s="9" t="s">
-        <v>82</v>
-      </c>
-      <c r="F221" s="9" t="s">
-        <v>149</v>
+      <c r="B221" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C221" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="D221" s="11">
+        <v>11</v>
+      </c>
+      <c r="E221" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="F221" s="5" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="222" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B222" s="9" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="C222" s="9" t="s">
         <v>91</v>
@@ -4956,47 +4964,62 @@
         <v>82</v>
       </c>
       <c r="F222" s="9" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="223" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B223" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="C223" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="D223" s="11"/>
+      <c r="E223" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="F223" s="9" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="224" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B224" s="9" t="s">
         <v>83</v>
       </c>
-      <c r="C223" s="9" t="s">
+      <c r="C224" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="D223" s="11">
-        <v>2</v>
-      </c>
-      <c r="E223" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="F223" s="5" t="s">
+      <c r="D224" s="11">
+        <v>2</v>
+      </c>
+      <c r="E224" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="F224" s="5" t="s">
         <v>152</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="B213:F213"/>
+    <mergeCell ref="B21:F21"/>
+    <mergeCell ref="B2:F2"/>
+    <mergeCell ref="B4:F4"/>
+    <mergeCell ref="B32:F32"/>
+    <mergeCell ref="B57:F57"/>
     <mergeCell ref="B116:F116"/>
-    <mergeCell ref="B193:F193"/>
-    <mergeCell ref="B132:F132"/>
+    <mergeCell ref="B194:F194"/>
+    <mergeCell ref="B133:F133"/>
     <mergeCell ref="B46:F46"/>
     <mergeCell ref="B67:F67"/>
     <mergeCell ref="B76:F76"/>
     <mergeCell ref="B86:F86"/>
     <mergeCell ref="B97:F97"/>
     <mergeCell ref="B107:F107"/>
-    <mergeCell ref="B21:F21"/>
-    <mergeCell ref="B2:F2"/>
-    <mergeCell ref="B4:F4"/>
-    <mergeCell ref="B32:F32"/>
-    <mergeCell ref="B57:F57"/>
-    <mergeCell ref="B142:F142"/>
-    <mergeCell ref="B153:F153"/>
-    <mergeCell ref="B170:F170"/>
-    <mergeCell ref="B180:F180"/>
-    <mergeCell ref="B212:F212"/>
+    <mergeCell ref="B143:F143"/>
+    <mergeCell ref="B154:F154"/>
+    <mergeCell ref="B171:F171"/>
+    <mergeCell ref="B181:F181"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Completed CURD for products
</commit_message>
<xml_diff>
--- a/Database Schema/Shopping_Database.xlsx
+++ b/Database Schema/Shopping_Database.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\eShoppingAdmin\Database Schema\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{467B0103-3689-41ED-8627-EB4810D2B7D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{161FE019-61D3-4F86-8297-96EF1F36E247}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{23AB6FBB-2C3C-4DC6-A36A-5E0C15916A1A}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="929" uniqueCount="184">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="899" uniqueCount="181">
   <si>
     <t>Users</t>
   </si>
@@ -389,9 +389,6 @@
     <t>required, foreign key</t>
   </si>
   <si>
-    <t>Table : ProductImages</t>
-  </si>
-  <si>
     <t>Table : ProductReview</t>
   </si>
   <si>
@@ -452,12 +449,6 @@
     <t>Date and Time when product is updated</t>
   </si>
   <si>
-    <t>Date and Time when pro. image is added</t>
-  </si>
-  <si>
-    <t>Date and Time when pro. image is updated</t>
-  </si>
-  <si>
     <t>Date and Time when review is added</t>
   </si>
   <si>
@@ -560,15 +551,9 @@
     <t>ProductColorIds</t>
   </si>
   <si>
-    <t>ProductImageIds</t>
-  </si>
-  <si>
     <t>optional set of foreign key</t>
   </si>
   <si>
-    <t>ImageURL</t>
-  </si>
-  <si>
     <t>productImageId</t>
   </si>
   <si>
@@ -588,6 +573,12 @@
   </si>
   <si>
     <t>SubCategoryId</t>
+  </si>
+  <si>
+    <t>text</t>
+  </si>
+  <si>
+    <t>optional set of name of image</t>
   </si>
 </sst>
 </file>
@@ -1975,11 +1966,6 @@
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="R3:T3"/>
-    <mergeCell ref="R12:T12"/>
-    <mergeCell ref="R24:T24"/>
-    <mergeCell ref="B3:D3"/>
-    <mergeCell ref="B16:D16"/>
     <mergeCell ref="B31:D31"/>
     <mergeCell ref="B26:D26"/>
     <mergeCell ref="N14:P14"/>
@@ -1991,6 +1977,11 @@
     <mergeCell ref="F13:H13"/>
     <mergeCell ref="F17:H17"/>
     <mergeCell ref="N3:P3"/>
+    <mergeCell ref="R3:T3"/>
+    <mergeCell ref="R12:T12"/>
+    <mergeCell ref="R24:T24"/>
+    <mergeCell ref="B3:D3"/>
+    <mergeCell ref="B16:D16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1999,10 +1990,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE0C0E27-F398-4128-B7EC-E6C5B9DA9B0B}">
-  <dimension ref="B2:AE224"/>
+  <dimension ref="B2:AE214"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A139" workbookViewId="0">
-      <selection activeCell="D149" sqref="D149"/>
+    <sheetView tabSelected="1" topLeftCell="A109" workbookViewId="0">
+      <selection activeCell="H125" sqref="H125"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2114,7 +2105,7 @@
         <v>81</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
     </row>
     <row r="11" spans="2:6" x14ac:dyDescent="0.3">
@@ -2263,7 +2254,7 @@
         <v>81</v>
       </c>
       <c r="F19" s="5" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
     </row>
     <row r="21" spans="2:7" ht="21" x14ac:dyDescent="0.4">
@@ -2341,7 +2332,7 @@
         <v>81</v>
       </c>
       <c r="F26" s="5" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
     </row>
     <row r="27" spans="2:7" x14ac:dyDescent="0.3">
@@ -2405,7 +2396,7 @@
         <v>81</v>
       </c>
       <c r="F30" s="5" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
     </row>
     <row r="32" spans="2:7" ht="21" x14ac:dyDescent="0.4">
@@ -2504,7 +2495,7 @@
     </row>
     <row r="39" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B39" s="5" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="C39" s="5" t="s">
         <v>1</v>
@@ -2516,7 +2507,7 @@
         <v>81</v>
       </c>
       <c r="F39" s="5" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
     </row>
     <row r="40" spans="2:6" x14ac:dyDescent="0.3">
@@ -2597,12 +2588,12 @@
         <v>81</v>
       </c>
       <c r="F44" s="5" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
     </row>
     <row r="46" spans="2:6" ht="21" x14ac:dyDescent="0.4">
       <c r="B46" s="17" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="C46" s="17"/>
       <c r="D46" s="17"/>
@@ -2674,7 +2665,7 @@
         <v>81</v>
       </c>
       <c r="F51" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
     </row>
     <row r="52" spans="2:31" x14ac:dyDescent="0.3">
@@ -2691,7 +2682,7 @@
         <v>81</v>
       </c>
       <c r="F52" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
     </row>
     <row r="53" spans="2:31" x14ac:dyDescent="0.3">
@@ -2706,7 +2697,7 @@
         <v>82</v>
       </c>
       <c r="F53" s="5" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
     </row>
     <row r="54" spans="2:31" x14ac:dyDescent="0.3">
@@ -2721,7 +2712,7 @@
         <v>82</v>
       </c>
       <c r="F54" s="5" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
     </row>
     <row r="55" spans="2:31" x14ac:dyDescent="0.3">
@@ -2738,7 +2729,7 @@
         <v>81</v>
       </c>
       <c r="F55" s="5" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
     </row>
     <row r="57" spans="2:31" ht="21" x14ac:dyDescent="0.4">
@@ -2831,7 +2822,7 @@
         <v>82</v>
       </c>
       <c r="F63" s="5" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
     </row>
     <row r="64" spans="2:31" x14ac:dyDescent="0.3">
@@ -2846,7 +2837,7 @@
         <v>82</v>
       </c>
       <c r="F64" s="5" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
     </row>
     <row r="65" spans="2:31" x14ac:dyDescent="0.3">
@@ -2863,7 +2854,7 @@
         <v>81</v>
       </c>
       <c r="F65" s="5" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
     </row>
     <row r="67" spans="2:31" ht="21" x14ac:dyDescent="0.4">
@@ -2939,7 +2930,7 @@
         <v>82</v>
       </c>
       <c r="F72" s="5" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
     </row>
     <row r="73" spans="2:31" x14ac:dyDescent="0.3">
@@ -2954,7 +2945,7 @@
         <v>82</v>
       </c>
       <c r="F73" s="5" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
     </row>
     <row r="74" spans="2:31" x14ac:dyDescent="0.3">
@@ -2971,7 +2962,7 @@
         <v>81</v>
       </c>
       <c r="F74" s="5" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
     </row>
     <row r="76" spans="2:31" ht="21" x14ac:dyDescent="0.4">
@@ -3020,7 +3011,7 @@
     </row>
     <row r="80" spans="2:31" x14ac:dyDescent="0.3">
       <c r="B80" s="5" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="C80" s="5" t="s">
         <v>2</v>
@@ -3037,7 +3028,7 @@
     </row>
     <row r="81" spans="2:31" x14ac:dyDescent="0.3">
       <c r="B81" s="9" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="C81" s="9" t="s">
         <v>2</v>
@@ -3049,12 +3040,12 @@
         <v>82</v>
       </c>
       <c r="F81" s="9" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
     </row>
     <row r="82" spans="2:31" x14ac:dyDescent="0.3">
       <c r="B82" s="9" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C82" s="9" t="s">
         <v>91</v>
@@ -3064,12 +3055,12 @@
         <v>82</v>
       </c>
       <c r="F82" s="9" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="83" spans="2:31" x14ac:dyDescent="0.3">
       <c r="B83" s="9" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C83" s="9" t="s">
         <v>91</v>
@@ -3079,7 +3070,7 @@
         <v>82</v>
       </c>
       <c r="F83" s="9" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="AC83" s="5"/>
       <c r="AD83" s="5"/>
@@ -3099,7 +3090,7 @@
         <v>81</v>
       </c>
       <c r="F84" s="5" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="AC84" s="5"/>
       <c r="AD84" s="5"/>
@@ -3168,7 +3159,7 @@
     </row>
     <row r="91" spans="2:31" x14ac:dyDescent="0.3">
       <c r="B91" s="5" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="C91" s="5" t="s">
         <v>2</v>
@@ -3186,7 +3177,7 @@
     </row>
     <row r="92" spans="2:31" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B92" s="9" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="C92" s="9" t="s">
         <v>2</v>
@@ -3198,12 +3189,12 @@
         <v>82</v>
       </c>
       <c r="F92" s="9" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
     </row>
     <row r="93" spans="2:31" x14ac:dyDescent="0.3">
       <c r="B93" s="9" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C93" s="9" t="s">
         <v>91</v>
@@ -3213,12 +3204,12 @@
         <v>82</v>
       </c>
       <c r="F93" s="9" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
     </row>
     <row r="94" spans="2:31" x14ac:dyDescent="0.3">
       <c r="B94" s="9" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C94" s="9" t="s">
         <v>91</v>
@@ -3228,7 +3219,7 @@
         <v>82</v>
       </c>
       <c r="F94" s="9" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
     </row>
     <row r="95" spans="2:31" x14ac:dyDescent="0.3">
@@ -3245,7 +3236,7 @@
         <v>81</v>
       </c>
       <c r="F95" s="5" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
     </row>
     <row r="96" spans="2:31" x14ac:dyDescent="0.3">
@@ -3318,7 +3309,7 @@
     </row>
     <row r="102" spans="2:31" x14ac:dyDescent="0.3">
       <c r="B102" s="5" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="C102" s="5" t="s">
         <v>2</v>
@@ -3335,7 +3326,7 @@
     </row>
     <row r="103" spans="2:31" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B103" s="9" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C103" s="9" t="s">
         <v>91</v>
@@ -3345,12 +3336,12 @@
         <v>82</v>
       </c>
       <c r="F103" s="9" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="104" spans="2:31" x14ac:dyDescent="0.3">
       <c r="B104" s="9" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C104" s="9" t="s">
         <v>91</v>
@@ -3360,7 +3351,7 @@
         <v>82</v>
       </c>
       <c r="F104" s="9" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="105" spans="2:31" x14ac:dyDescent="0.3">
@@ -3377,7 +3368,7 @@
         <v>81</v>
       </c>
       <c r="F105" s="5" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
     </row>
     <row r="107" spans="2:31" ht="21" x14ac:dyDescent="0.4">
@@ -3444,7 +3435,7 @@
     </row>
     <row r="112" spans="2:31" x14ac:dyDescent="0.3">
       <c r="B112" s="9" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C112" s="9" t="s">
         <v>91</v>
@@ -3454,12 +3445,12 @@
         <v>82</v>
       </c>
       <c r="F112" s="9" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="113" spans="2:31" x14ac:dyDescent="0.3">
       <c r="B113" s="9" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C113" s="9" t="s">
         <v>91</v>
@@ -3469,7 +3460,7 @@
         <v>82</v>
       </c>
       <c r="F113" s="9" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="114" spans="2:31" x14ac:dyDescent="0.3">
@@ -3486,7 +3477,7 @@
         <v>81</v>
       </c>
       <c r="F114" s="5" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
     </row>
     <row r="116" spans="2:31" ht="21" x14ac:dyDescent="0.4">
@@ -3569,7 +3560,7 @@
     </row>
     <row r="122" spans="2:31" x14ac:dyDescent="0.3">
       <c r="B122" s="5" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
       <c r="C122" s="5" t="s">
         <v>1</v>
@@ -3586,7 +3577,7 @@
     </row>
     <row r="123" spans="2:31" x14ac:dyDescent="0.3">
       <c r="B123" s="5" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="C123" s="5" t="s">
         <v>2</v>
@@ -3598,12 +3589,12 @@
         <v>81</v>
       </c>
       <c r="F123" s="5" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
     </row>
     <row r="124" spans="2:31" x14ac:dyDescent="0.3">
       <c r="B124" s="5" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="C124" s="5" t="s">
         <v>2</v>
@@ -3615,24 +3606,22 @@
         <v>81</v>
       </c>
       <c r="F124" s="5" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
     </row>
     <row r="125" spans="2:31" x14ac:dyDescent="0.3">
       <c r="B125" s="9" t="s">
-        <v>174</v>
+        <v>36</v>
       </c>
       <c r="C125" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="D125" s="11">
-        <v>100</v>
-      </c>
+        <v>179</v>
+      </c>
+      <c r="D125" s="11"/>
       <c r="E125" s="9" t="s">
         <v>81</v>
       </c>
       <c r="F125" s="9" t="s">
-        <v>175</v>
+        <v>180</v>
       </c>
     </row>
     <row r="126" spans="2:31" x14ac:dyDescent="0.3">
@@ -3671,7 +3660,7 @@
     </row>
     <row r="128" spans="2:31" x14ac:dyDescent="0.3">
       <c r="B128" s="9" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="C128" s="9" t="s">
         <v>1</v>
@@ -3688,7 +3677,7 @@
     </row>
     <row r="129" spans="2:31" x14ac:dyDescent="0.3">
       <c r="B129" s="9" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C129" s="9" t="s">
         <v>91</v>
@@ -3698,13 +3687,13 @@
         <v>82</v>
       </c>
       <c r="F129" s="9" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="AE129" s="10"/>
     </row>
     <row r="130" spans="2:31" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B130" s="9" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C130" s="9" t="s">
         <v>91</v>
@@ -3714,7 +3703,7 @@
         <v>82</v>
       </c>
       <c r="F130" s="9" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="131" spans="2:31" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -3731,7 +3720,7 @@
         <v>81</v>
       </c>
       <c r="F131" s="5" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
     </row>
     <row r="133" spans="2:31" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.4">
@@ -3796,40 +3785,42 @@
     </row>
     <row r="138" spans="2:31" x14ac:dyDescent="0.3">
       <c r="B138" s="5" t="s">
-        <v>176</v>
+        <v>39</v>
       </c>
       <c r="C138" s="5" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D138" s="11">
+        <v>11</v>
+      </c>
+      <c r="E138" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="F138" s="5" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="139" spans="2:31" x14ac:dyDescent="0.3">
+      <c r="B139" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="C139" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D139" s="11">
         <v>150</v>
       </c>
-      <c r="E138" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="F138" s="5" t="s">
+      <c r="E139" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="F139" s="5" t="s">
         <v>115</v>
-      </c>
-    </row>
-    <row r="139" spans="2:31" x14ac:dyDescent="0.3">
-      <c r="B139" s="9" t="s">
-        <v>131</v>
-      </c>
-      <c r="C139" s="9" t="s">
-        <v>91</v>
-      </c>
-      <c r="D139" s="11"/>
-      <c r="E139" s="9" t="s">
-        <v>82</v>
-      </c>
-      <c r="F139" s="9" t="s">
-        <v>138</v>
       </c>
       <c r="AE139" s="10"/>
     </row>
     <row r="140" spans="2:31" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B140" s="9" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="C140" s="9" t="s">
         <v>91</v>
@@ -3839,72 +3830,70 @@
         <v>82</v>
       </c>
       <c r="F140" s="9" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
     </row>
     <row r="141" spans="2:31" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B141" s="9" t="s">
+        <v>128</v>
+      </c>
+      <c r="C141" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="D141" s="11"/>
+      <c r="E141" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="F141" s="9" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="142" spans="2:31" x14ac:dyDescent="0.3">
+      <c r="B142" s="9" t="s">
         <v>83</v>
       </c>
-      <c r="C141" s="9" t="s">
+      <c r="C142" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="D141" s="11">
-        <v>2</v>
-      </c>
-      <c r="E141" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="F141" s="5" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="143" spans="2:31" ht="21" x14ac:dyDescent="0.4">
-      <c r="B143" s="17" t="s">
-        <v>118</v>
-      </c>
-      <c r="C143" s="17"/>
-      <c r="D143" s="17"/>
-      <c r="E143" s="17"/>
-      <c r="F143" s="17"/>
-    </row>
-    <row r="145" spans="2:31" ht="18" x14ac:dyDescent="0.35">
-      <c r="B145" s="12" t="s">
+      <c r="D142" s="11">
+        <v>2</v>
+      </c>
+      <c r="E142" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="F142" s="5" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="144" spans="2:31" ht="21" x14ac:dyDescent="0.4">
+      <c r="B144" s="17" t="s">
+        <v>119</v>
+      </c>
+      <c r="C144" s="17"/>
+      <c r="D144" s="17"/>
+      <c r="E144" s="17"/>
+      <c r="F144" s="17"/>
+    </row>
+    <row r="146" spans="2:31" ht="18" x14ac:dyDescent="0.35">
+      <c r="B146" s="12" t="s">
         <v>74</v>
       </c>
-      <c r="C145" s="12" t="s">
+      <c r="C146" s="12" t="s">
         <v>75</v>
       </c>
-      <c r="D145" s="13" t="s">
+      <c r="D146" s="13" t="s">
         <v>76</v>
       </c>
-      <c r="E145" s="12" t="s">
+      <c r="E146" s="12" t="s">
         <v>77</v>
       </c>
-      <c r="F145" s="12" t="s">
+      <c r="F146" s="12" t="s">
         <v>78</v>
-      </c>
-    </row>
-    <row r="146" spans="2:31" x14ac:dyDescent="0.3">
-      <c r="B146" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C146" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="D146" s="11">
-        <v>11</v>
-      </c>
-      <c r="E146" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="F146" s="5" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="147" spans="2:31" x14ac:dyDescent="0.3">
       <c r="B147" s="5" t="s">
-        <v>35</v>
+        <v>11</v>
       </c>
       <c r="C147" s="5" t="s">
         <v>1</v>
@@ -3916,12 +3905,12 @@
         <v>81</v>
       </c>
       <c r="F147" s="5" t="s">
-        <v>116</v>
+        <v>84</v>
       </c>
     </row>
     <row r="148" spans="2:31" x14ac:dyDescent="0.3">
       <c r="B148" s="5" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="C148" s="5" t="s">
         <v>1</v>
@@ -3933,226 +3922,226 @@
         <v>81</v>
       </c>
       <c r="F148" s="5" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
     </row>
     <row r="149" spans="2:31" x14ac:dyDescent="0.3">
-      <c r="B149" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="C149" s="5" t="s">
-        <v>2</v>
+      <c r="B149" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="C149" s="9" t="s">
+        <v>1</v>
       </c>
       <c r="D149" s="11">
-        <v>150</v>
+        <v>11</v>
       </c>
       <c r="E149" s="5" t="s">
         <v>81</v>
       </c>
       <c r="F149" s="5" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="150" spans="2:31" x14ac:dyDescent="0.3">
+      <c r="B150" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="C150" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D150" s="11">
+        <v>100</v>
+      </c>
+      <c r="E150" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="F150" s="5" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="150" spans="2:31" x14ac:dyDescent="0.3">
-      <c r="B150" s="9" t="s">
-        <v>131</v>
-      </c>
-      <c r="C150" s="9" t="s">
+    <row r="151" spans="2:31" x14ac:dyDescent="0.3">
+      <c r="B151" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="C151" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="D151" s="11">
+        <v>11</v>
+      </c>
+      <c r="E151" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="F151" s="5" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="152" spans="2:31" x14ac:dyDescent="0.3">
+      <c r="B152" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="C152" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="D152" s="11">
+        <v>11</v>
+      </c>
+      <c r="E152" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="F152" s="5" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="153" spans="2:31" x14ac:dyDescent="0.3">
+      <c r="B153" s="9" t="s">
+        <v>172</v>
+      </c>
+      <c r="C153" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="D153" s="11">
+        <v>11</v>
+      </c>
+      <c r="E153" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="F153" s="9" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="154" spans="2:31" x14ac:dyDescent="0.3">
+      <c r="B154" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="C154" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="D154" s="11">
+        <v>11</v>
+      </c>
+      <c r="E154" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="F154" s="5" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="155" spans="2:31" x14ac:dyDescent="0.3">
+      <c r="B155" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="C155" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="D155" s="11">
+        <v>11</v>
+      </c>
+      <c r="E155" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="F155" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="AE155" s="10"/>
+    </row>
+    <row r="156" spans="2:31" x14ac:dyDescent="0.3">
+      <c r="B156" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="C156" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="D156" s="11">
+        <v>11</v>
+      </c>
+      <c r="E156" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="F156" s="5" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="157" spans="2:31" x14ac:dyDescent="0.3">
+      <c r="B157" s="9" t="s">
+        <v>130</v>
+      </c>
+      <c r="C157" s="9" t="s">
         <v>91</v>
       </c>
-      <c r="D150" s="11"/>
-      <c r="E150" s="9" t="s">
+      <c r="D157" s="11"/>
+      <c r="E157" s="9" t="s">
         <v>82</v>
       </c>
-      <c r="F150" s="9" t="s">
+      <c r="F157" s="9" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="158" spans="2:31" x14ac:dyDescent="0.3">
+      <c r="B158" s="9" t="s">
+        <v>128</v>
+      </c>
+      <c r="C158" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="D158" s="11"/>
+      <c r="E158" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="F158" s="9" t="s">
         <v>140</v>
-      </c>
-    </row>
-    <row r="151" spans="2:31" x14ac:dyDescent="0.3">
-      <c r="B151" s="9" t="s">
-        <v>129</v>
-      </c>
-      <c r="C151" s="9" t="s">
-        <v>91</v>
-      </c>
-      <c r="D151" s="11"/>
-      <c r="E151" s="9" t="s">
-        <v>82</v>
-      </c>
-      <c r="F151" s="9" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="152" spans="2:31" x14ac:dyDescent="0.3">
-      <c r="B152" s="9" t="s">
-        <v>83</v>
-      </c>
-      <c r="C152" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="D152" s="11">
-        <v>2</v>
-      </c>
-      <c r="E152" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="F152" s="5" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="154" spans="2:31" ht="21" x14ac:dyDescent="0.4">
-      <c r="B154" s="17" t="s">
-        <v>120</v>
-      </c>
-      <c r="C154" s="17"/>
-      <c r="D154" s="17"/>
-      <c r="E154" s="17"/>
-      <c r="F154" s="17"/>
-    </row>
-    <row r="155" spans="2:31" x14ac:dyDescent="0.3">
-      <c r="AE155" s="10"/>
-    </row>
-    <row r="156" spans="2:31" ht="18" x14ac:dyDescent="0.35">
-      <c r="B156" s="12" t="s">
-        <v>74</v>
-      </c>
-      <c r="C156" s="12" t="s">
-        <v>75</v>
-      </c>
-      <c r="D156" s="13" t="s">
-        <v>76</v>
-      </c>
-      <c r="E156" s="12" t="s">
-        <v>77</v>
-      </c>
-      <c r="F156" s="12" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="157" spans="2:31" x14ac:dyDescent="0.3">
-      <c r="B157" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C157" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="D157" s="11">
-        <v>11</v>
-      </c>
-      <c r="E157" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="F157" s="5" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="158" spans="2:31" x14ac:dyDescent="0.3">
-      <c r="B158" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="C158" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="D158" s="11">
-        <v>11</v>
-      </c>
-      <c r="E158" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="F158" s="5" t="s">
-        <v>116</v>
       </c>
     </row>
     <row r="159" spans="2:31" x14ac:dyDescent="0.3">
       <c r="B159" s="9" t="s">
-        <v>18</v>
+        <v>83</v>
       </c>
       <c r="C159" s="9" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D159" s="11">
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="E159" s="5" t="s">
         <v>81</v>
       </c>
       <c r="F159" s="5" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="160" spans="2:31" x14ac:dyDescent="0.3">
-      <c r="B160" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="C160" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="D160" s="11">
-        <v>100</v>
-      </c>
-      <c r="E160" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="F160" s="5" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="161" spans="2:31" x14ac:dyDescent="0.3">
-      <c r="B161" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="C161" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="D161" s="11">
-        <v>11</v>
-      </c>
-      <c r="E161" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="F161" s="5" t="s">
-        <v>116</v>
-      </c>
+        <v>149</v>
+      </c>
+    </row>
+    <row r="161" spans="2:31" ht="21" x14ac:dyDescent="0.4">
+      <c r="B161" s="17" t="s">
+        <v>120</v>
+      </c>
+      <c r="C161" s="17"/>
+      <c r="D161" s="17"/>
+      <c r="E161" s="17"/>
+      <c r="F161" s="17"/>
     </row>
     <row r="162" spans="2:31" x14ac:dyDescent="0.3">
-      <c r="B162" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="C162" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="D162" s="11">
-        <v>11</v>
-      </c>
-      <c r="E162" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="F162" s="5" t="s">
-        <v>116</v>
-      </c>
       <c r="AE162" s="10"/>
     </row>
-    <row r="163" spans="2:31" x14ac:dyDescent="0.3">
-      <c r="B163" s="9" t="s">
-        <v>177</v>
-      </c>
-      <c r="C163" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="D163" s="11">
-        <v>11</v>
-      </c>
-      <c r="E163" s="9" t="s">
-        <v>81</v>
-      </c>
-      <c r="F163" s="9" t="s">
-        <v>116</v>
+    <row r="163" spans="2:31" ht="18" x14ac:dyDescent="0.35">
+      <c r="B163" s="12" t="s">
+        <v>74</v>
+      </c>
+      <c r="C163" s="12" t="s">
+        <v>75</v>
+      </c>
+      <c r="D163" s="13" t="s">
+        <v>76</v>
+      </c>
+      <c r="E163" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="F163" s="12" t="s">
+        <v>78</v>
       </c>
       <c r="AE163" s="10"/>
     </row>
     <row r="164" spans="2:31" x14ac:dyDescent="0.3">
       <c r="B164" s="5" t="s">
-        <v>53</v>
+        <v>11</v>
       </c>
       <c r="C164" s="5" t="s">
         <v>1</v>
@@ -4164,12 +4153,12 @@
         <v>81</v>
       </c>
       <c r="F164" s="5" t="s">
-        <v>115</v>
+        <v>84</v>
       </c>
     </row>
     <row r="165" spans="2:31" x14ac:dyDescent="0.3">
       <c r="B165" s="5" t="s">
-        <v>52</v>
+        <v>35</v>
       </c>
       <c r="C165" s="5" t="s">
         <v>1</v>
@@ -4181,14 +4170,14 @@
         <v>81</v>
       </c>
       <c r="F165" s="5" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
     </row>
     <row r="166" spans="2:31" x14ac:dyDescent="0.3">
-      <c r="B166" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="C166" s="5" t="s">
+      <c r="B166" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="C166" s="9" t="s">
         <v>1</v>
       </c>
       <c r="D166" s="11">
@@ -4198,12 +4187,12 @@
         <v>81</v>
       </c>
       <c r="F166" s="5" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
     </row>
     <row r="167" spans="2:31" x14ac:dyDescent="0.3">
       <c r="B167" s="9" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C167" s="9" t="s">
         <v>91</v>
@@ -4213,12 +4202,12 @@
         <v>82</v>
       </c>
       <c r="F167" s="9" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="168" spans="2:31" x14ac:dyDescent="0.3">
       <c r="B168" s="9" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C168" s="9" t="s">
         <v>91</v>
@@ -4228,7 +4217,7 @@
         <v>82</v>
       </c>
       <c r="F168" s="9" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="169" spans="2:31" x14ac:dyDescent="0.3">
@@ -4245,7 +4234,7 @@
         <v>81</v>
       </c>
       <c r="F169" s="5" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
     </row>
     <row r="171" spans="2:31" ht="21" x14ac:dyDescent="0.4">
@@ -4293,7 +4282,7 @@
     </row>
     <row r="175" spans="2:31" x14ac:dyDescent="0.3">
       <c r="B175" s="5" t="s">
-        <v>35</v>
+        <v>18</v>
       </c>
       <c r="C175" s="5" t="s">
         <v>1</v>
@@ -4310,147 +4299,147 @@
       <c r="AE175" s="10"/>
     </row>
     <row r="176" spans="2:31" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B176" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="C176" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="D176" s="11">
-        <v>11</v>
-      </c>
+      <c r="B176" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="C176" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="D176" s="11"/>
       <c r="E176" s="5" t="s">
         <v>81</v>
       </c>
       <c r="F176" s="5" t="s">
-        <v>116</v>
+        <v>122</v>
       </c>
     </row>
     <row r="177" spans="2:31" x14ac:dyDescent="0.3">
-      <c r="B177" s="9" t="s">
-        <v>131</v>
-      </c>
-      <c r="C177" s="9" t="s">
+      <c r="B177" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="C177" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="D177" s="11">
+        <v>11</v>
+      </c>
+      <c r="E177" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="F177" s="5" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="178" spans="2:31" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B178" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="C178" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="D178" s="11">
+        <v>11</v>
+      </c>
+      <c r="E178" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="F178" s="5" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="179" spans="2:31" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B179" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="C179" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="D179" s="11"/>
+      <c r="E179" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="F179" s="5" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="180" spans="2:31" x14ac:dyDescent="0.3">
+      <c r="B180" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="C180" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="D180" s="11">
+        <v>11</v>
+      </c>
+      <c r="E180" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="F180" s="5" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="181" spans="2:31" x14ac:dyDescent="0.3">
+      <c r="B181" s="9" t="s">
+        <v>128</v>
+      </c>
+      <c r="C181" s="9" t="s">
         <v>91</v>
       </c>
-      <c r="D177" s="11"/>
-      <c r="E177" s="9" t="s">
+      <c r="D181" s="11"/>
+      <c r="E181" s="9" t="s">
         <v>82</v>
       </c>
-      <c r="F177" s="9" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="178" spans="2:31" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B178" s="9" t="s">
-        <v>129</v>
-      </c>
-      <c r="C178" s="9" t="s">
-        <v>91</v>
-      </c>
-      <c r="D178" s="11"/>
-      <c r="E178" s="9" t="s">
-        <v>82</v>
-      </c>
-      <c r="F178" s="9" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="179" spans="2:31" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B179" s="9" t="s">
+      <c r="F181" s="9" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="182" spans="2:31" x14ac:dyDescent="0.3">
+      <c r="B182" s="9" t="s">
         <v>83</v>
       </c>
-      <c r="C179" s="9" t="s">
+      <c r="C182" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="D179" s="11">
-        <v>2</v>
-      </c>
-      <c r="E179" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="F179" s="5" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="181" spans="2:31" ht="21" x14ac:dyDescent="0.4">
-      <c r="B181" s="17" t="s">
-        <v>122</v>
-      </c>
-      <c r="C181" s="17"/>
-      <c r="D181" s="17"/>
-      <c r="E181" s="17"/>
-      <c r="F181" s="17"/>
-    </row>
-    <row r="183" spans="2:31" ht="18" x14ac:dyDescent="0.35">
-      <c r="B183" s="12" t="s">
+      <c r="D182" s="11">
+        <v>2</v>
+      </c>
+      <c r="E182" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="F182" s="5" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="184" spans="2:31" ht="21" x14ac:dyDescent="0.4">
+      <c r="B184" s="17" t="s">
+        <v>124</v>
+      </c>
+      <c r="C184" s="17"/>
+      <c r="D184" s="17"/>
+      <c r="E184" s="17"/>
+      <c r="F184" s="17"/>
+    </row>
+    <row r="186" spans="2:31" ht="18" x14ac:dyDescent="0.35">
+      <c r="B186" s="12" t="s">
         <v>74</v>
       </c>
-      <c r="C183" s="12" t="s">
+      <c r="C186" s="12" t="s">
         <v>75</v>
       </c>
-      <c r="D183" s="13" t="s">
+      <c r="D186" s="13" t="s">
         <v>76</v>
       </c>
-      <c r="E183" s="12" t="s">
+      <c r="E186" s="12" t="s">
         <v>77</v>
       </c>
-      <c r="F183" s="12" t="s">
+      <c r="F186" s="12" t="s">
         <v>78</v>
-      </c>
-    </row>
-    <row r="184" spans="2:31" x14ac:dyDescent="0.3">
-      <c r="B184" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C184" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="D184" s="11">
-        <v>11</v>
-      </c>
-      <c r="E184" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="F184" s="5" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="185" spans="2:31" x14ac:dyDescent="0.3">
-      <c r="B185" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="C185" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="D185" s="11">
-        <v>11</v>
-      </c>
-      <c r="E185" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="F185" s="5" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="186" spans="2:31" x14ac:dyDescent="0.3">
-      <c r="B186" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="C186" s="5" t="s">
-        <v>91</v>
-      </c>
-      <c r="D186" s="11"/>
-      <c r="E186" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="F186" s="5" t="s">
-        <v>123</v>
       </c>
     </row>
     <row r="187" spans="2:31" x14ac:dyDescent="0.3">
       <c r="B187" s="5" t="s">
-        <v>57</v>
+        <v>11</v>
       </c>
       <c r="C187" s="5" t="s">
         <v>1</v>
@@ -4462,12 +4451,12 @@
         <v>81</v>
       </c>
       <c r="F187" s="5" t="s">
-        <v>115</v>
+        <v>84</v>
       </c>
     </row>
     <row r="188" spans="2:31" x14ac:dyDescent="0.3">
       <c r="B188" s="5" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="C188" s="5" t="s">
         <v>1</v>
@@ -4479,103 +4468,149 @@
         <v>81</v>
       </c>
       <c r="F188" s="5" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
     </row>
     <row r="189" spans="2:31" x14ac:dyDescent="0.3">
       <c r="B189" s="5" t="s">
-        <v>67</v>
+        <v>35</v>
       </c>
       <c r="C189" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="D189" s="11"/>
+        <v>1</v>
+      </c>
+      <c r="D189" s="11">
+        <v>11</v>
+      </c>
       <c r="E189" s="5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F189" s="5" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
     </row>
     <row r="190" spans="2:31" x14ac:dyDescent="0.3">
       <c r="B190" s="5" t="s">
-        <v>65</v>
+        <v>29</v>
       </c>
       <c r="C190" s="5" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D190" s="11">
-        <v>11</v>
+        <v>50</v>
       </c>
       <c r="E190" s="5" t="s">
         <v>81</v>
       </c>
       <c r="F190" s="5" t="s">
-        <v>124</v>
+        <v>115</v>
       </c>
       <c r="AE190" s="10"/>
     </row>
     <row r="191" spans="2:31" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B191" s="9" t="s">
-        <v>129</v>
-      </c>
-      <c r="C191" s="9" t="s">
-        <v>91</v>
-      </c>
-      <c r="D191" s="11"/>
-      <c r="E191" s="9" t="s">
-        <v>82</v>
-      </c>
-      <c r="F191" s="9" t="s">
-        <v>146</v>
+      <c r="B191" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="C191" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D191" s="11">
+        <v>50</v>
+      </c>
+      <c r="E191" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="F191" s="5" t="s">
+        <v>115</v>
       </c>
     </row>
     <row r="192" spans="2:31" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B192" s="9" t="s">
-        <v>83</v>
-      </c>
-      <c r="C192" s="9" t="s">
-        <v>3</v>
+      <c r="B192" s="5" t="s">
+        <v>176</v>
+      </c>
+      <c r="C192" s="5" t="s">
+        <v>2</v>
       </c>
       <c r="D192" s="11">
-        <v>2</v>
+        <v>100</v>
       </c>
       <c r="E192" s="5" t="s">
         <v>81</v>
       </c>
       <c r="F192" s="5" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="194" spans="2:6" ht="21" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B194" s="17" t="s">
-        <v>125</v>
-      </c>
-      <c r="C194" s="17"/>
-      <c r="D194" s="17"/>
-      <c r="E194" s="17"/>
-      <c r="F194" s="17"/>
-    </row>
-    <row r="196" spans="2:6" ht="18" x14ac:dyDescent="0.35">
-      <c r="B196" s="12" t="s">
-        <v>74</v>
-      </c>
-      <c r="C196" s="12" t="s">
-        <v>75</v>
-      </c>
-      <c r="D196" s="13" t="s">
-        <v>76</v>
-      </c>
-      <c r="E196" s="12" t="s">
-        <v>77</v>
-      </c>
-      <c r="F196" s="12" t="s">
-        <v>78</v>
+        <v>115</v>
+      </c>
+    </row>
+    <row r="193" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B193" s="5" t="s">
+        <v>173</v>
+      </c>
+      <c r="C193" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D193" s="11">
+        <v>50</v>
+      </c>
+      <c r="E193" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="F193" s="5" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="194" spans="2:6" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B194" s="9" t="s">
+        <v>174</v>
+      </c>
+      <c r="C194" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="D194" s="11">
+        <v>50</v>
+      </c>
+      <c r="E194" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="F194" s="9" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="195" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B195" s="5" t="s">
+        <v>175</v>
+      </c>
+      <c r="C195" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="D195" s="11">
+        <v>50</v>
+      </c>
+      <c r="E195" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="F195" s="5" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="196" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B196" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="C196" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="D196" s="11">
+        <v>11</v>
+      </c>
+      <c r="E196" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="F196" s="5" t="s">
+        <v>115</v>
       </c>
     </row>
     <row r="197" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B197" s="5" t="s">
-        <v>11</v>
+        <v>63</v>
       </c>
       <c r="C197" s="5" t="s">
         <v>1</v>
@@ -4587,12 +4622,12 @@
         <v>81</v>
       </c>
       <c r="F197" s="5" t="s">
-        <v>84</v>
+        <v>115</v>
       </c>
     </row>
     <row r="198" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B198" s="5" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="C198" s="5" t="s">
         <v>1</v>
@@ -4604,131 +4639,85 @@
         <v>81</v>
       </c>
       <c r="F198" s="5" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="199" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B199" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="C199" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="D199" s="11">
-        <v>11</v>
-      </c>
-      <c r="E199" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="F199" s="5" t="s">
-        <v>116</v>
+      <c r="B199" s="9" t="s">
+        <v>130</v>
+      </c>
+      <c r="C199" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="D199" s="11"/>
+      <c r="E199" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="F199" s="9" t="s">
+        <v>145</v>
       </c>
     </row>
     <row r="200" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B200" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="C200" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="D200" s="11">
-        <v>50</v>
-      </c>
-      <c r="E200" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="F200" s="5" t="s">
-        <v>115</v>
+      <c r="B200" s="9" t="s">
+        <v>128</v>
+      </c>
+      <c r="C200" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="D200" s="11"/>
+      <c r="E200" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="F200" s="9" t="s">
+        <v>144</v>
       </c>
     </row>
     <row r="201" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B201" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="C201" s="5" t="s">
-        <v>2</v>
+      <c r="B201" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="C201" s="9" t="s">
+        <v>3</v>
       </c>
       <c r="D201" s="11">
-        <v>50</v>
+        <v>2</v>
       </c>
       <c r="E201" s="5" t="s">
         <v>81</v>
       </c>
       <c r="F201" s="5" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="202" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B202" s="5" t="s">
-        <v>181</v>
-      </c>
-      <c r="C202" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="D202" s="11">
-        <v>100</v>
-      </c>
-      <c r="E202" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="F202" s="5" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="203" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B203" s="5" t="s">
-        <v>178</v>
-      </c>
-      <c r="C203" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="D203" s="11">
-        <v>50</v>
-      </c>
-      <c r="E203" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="F203" s="5" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="204" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B204" s="9" t="s">
-        <v>179</v>
-      </c>
-      <c r="C204" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="D204" s="11">
-        <v>50</v>
-      </c>
-      <c r="E204" s="9" t="s">
-        <v>81</v>
-      </c>
-      <c r="F204" s="9" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="205" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B205" s="5" t="s">
-        <v>180</v>
-      </c>
-      <c r="C205" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="D205" s="11">
-        <v>50</v>
-      </c>
-      <c r="E205" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="F205" s="5" t="s">
-        <v>115</v>
+        <v>149</v>
+      </c>
+    </row>
+    <row r="203" spans="2:6" ht="21" x14ac:dyDescent="0.4">
+      <c r="B203" s="17" t="s">
+        <v>125</v>
+      </c>
+      <c r="C203" s="17"/>
+      <c r="D203" s="17"/>
+      <c r="E203" s="17"/>
+      <c r="F203" s="17"/>
+    </row>
+    <row r="205" spans="2:6" ht="18" x14ac:dyDescent="0.35">
+      <c r="B205" s="12" t="s">
+        <v>74</v>
+      </c>
+      <c r="C205" s="12" t="s">
+        <v>75</v>
+      </c>
+      <c r="D205" s="13" t="s">
+        <v>76</v>
+      </c>
+      <c r="E205" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="F205" s="12" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="206" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B206" s="5" t="s">
-        <v>62</v>
+        <v>11</v>
       </c>
       <c r="C206" s="5" t="s">
         <v>1</v>
@@ -4740,12 +4729,12 @@
         <v>81</v>
       </c>
       <c r="F206" s="5" t="s">
-        <v>115</v>
+        <v>84</v>
       </c>
     </row>
     <row r="207" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B207" s="5" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="C207" s="5" t="s">
         <v>1</v>
@@ -4757,18 +4746,18 @@
         <v>81</v>
       </c>
       <c r="F207" s="5" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
     </row>
     <row r="208" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B208" s="5" t="s">
-        <v>64</v>
+        <v>20</v>
       </c>
       <c r="C208" s="5" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D208" s="11">
-        <v>11</v>
+        <v>50</v>
       </c>
       <c r="E208" s="5" t="s">
         <v>81</v>
@@ -4778,248 +4767,123 @@
       </c>
     </row>
     <row r="209" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B209" s="9" t="s">
-        <v>131</v>
-      </c>
-      <c r="C209" s="9" t="s">
+      <c r="B209" s="5" t="s">
+        <v>151</v>
+      </c>
+      <c r="C209" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="D209" s="11">
+        <v>11</v>
+      </c>
+      <c r="E209" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="F209" s="5" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="210" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B210" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C210" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="D210" s="11">
+        <v>11</v>
+      </c>
+      <c r="E210" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="F210" s="5" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="211" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B211" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C211" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="D211" s="11">
+        <v>11</v>
+      </c>
+      <c r="E211" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="F211" s="5" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="212" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B212" s="9" t="s">
+        <v>130</v>
+      </c>
+      <c r="C212" s="9" t="s">
         <v>91</v>
       </c>
-      <c r="D209" s="11"/>
-      <c r="E209" s="9" t="s">
+      <c r="D212" s="11"/>
+      <c r="E212" s="9" t="s">
         <v>82</v>
       </c>
-      <c r="F209" s="9" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="210" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B210" s="9" t="s">
-        <v>129</v>
-      </c>
-      <c r="C210" s="9" t="s">
+      <c r="F212" s="9" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="213" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B213" s="9" t="s">
+        <v>128</v>
+      </c>
+      <c r="C213" s="9" t="s">
         <v>91</v>
       </c>
-      <c r="D210" s="11"/>
-      <c r="E210" s="9" t="s">
+      <c r="D213" s="11"/>
+      <c r="E213" s="9" t="s">
         <v>82</v>
       </c>
-      <c r="F210" s="9" t="s">
+      <c r="F213" s="9" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="211" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B211" s="9" t="s">
+    <row r="214" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B214" s="9" t="s">
         <v>83</v>
       </c>
-      <c r="C211" s="9" t="s">
+      <c r="C214" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="D211" s="11">
-        <v>2</v>
-      </c>
-      <c r="E211" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="F211" s="5" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="213" spans="2:6" ht="21" x14ac:dyDescent="0.4">
-      <c r="B213" s="17" t="s">
-        <v>126</v>
-      </c>
-      <c r="C213" s="17"/>
-      <c r="D213" s="17"/>
-      <c r="E213" s="17"/>
-      <c r="F213" s="17"/>
-    </row>
-    <row r="215" spans="2:6" ht="18" x14ac:dyDescent="0.35">
-      <c r="B215" s="12" t="s">
-        <v>74</v>
-      </c>
-      <c r="C215" s="12" t="s">
-        <v>75</v>
-      </c>
-      <c r="D215" s="13" t="s">
-        <v>76</v>
-      </c>
-      <c r="E215" s="12" t="s">
-        <v>77</v>
-      </c>
-      <c r="F215" s="12" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="216" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B216" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C216" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="D216" s="11">
-        <v>11</v>
-      </c>
-      <c r="E216" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="F216" s="5" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="217" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B217" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="C217" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="D217" s="11">
-        <v>11</v>
-      </c>
-      <c r="E217" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="F217" s="5" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="218" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B218" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="C218" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="D218" s="11">
-        <v>50</v>
-      </c>
-      <c r="E218" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="F218" s="5" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="219" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B219" s="5" t="s">
-        <v>154</v>
-      </c>
-      <c r="C219" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="D219" s="11">
-        <v>11</v>
-      </c>
-      <c r="E219" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="F219" s="5" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="220" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B220" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="C220" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="D220" s="11">
-        <v>11</v>
-      </c>
-      <c r="E220" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="F220" s="5" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="221" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B221" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="C221" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="D221" s="11">
-        <v>11</v>
-      </c>
-      <c r="E221" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="F221" s="5" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="222" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B222" s="9" t="s">
-        <v>131</v>
-      </c>
-      <c r="C222" s="9" t="s">
-        <v>91</v>
-      </c>
-      <c r="D222" s="11"/>
-      <c r="E222" s="9" t="s">
-        <v>82</v>
-      </c>
-      <c r="F222" s="9" t="s">
+      <c r="D214" s="11">
+        <v>2</v>
+      </c>
+      <c r="E214" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="F214" s="5" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="223" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B223" s="9" t="s">
-        <v>129</v>
-      </c>
-      <c r="C223" s="9" t="s">
-        <v>91</v>
-      </c>
-      <c r="D223" s="11"/>
-      <c r="E223" s="9" t="s">
-        <v>82</v>
-      </c>
-      <c r="F223" s="9" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="224" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B224" s="9" t="s">
-        <v>83</v>
-      </c>
-      <c r="C224" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="D224" s="11">
-        <v>2</v>
-      </c>
-      <c r="E224" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="F224" s="5" t="s">
-        <v>152</v>
-      </c>
-    </row>
   </sheetData>
-  <mergeCells count="19">
-    <mergeCell ref="B213:F213"/>
+  <mergeCells count="18">
+    <mergeCell ref="B144:F144"/>
+    <mergeCell ref="B161:F161"/>
+    <mergeCell ref="B171:F171"/>
+    <mergeCell ref="B203:F203"/>
     <mergeCell ref="B21:F21"/>
     <mergeCell ref="B2:F2"/>
     <mergeCell ref="B4:F4"/>
     <mergeCell ref="B32:F32"/>
     <mergeCell ref="B57:F57"/>
     <mergeCell ref="B116:F116"/>
-    <mergeCell ref="B194:F194"/>
-    <mergeCell ref="B133:F133"/>
+    <mergeCell ref="B184:F184"/>
     <mergeCell ref="B46:F46"/>
     <mergeCell ref="B67:F67"/>
     <mergeCell ref="B76:F76"/>
     <mergeCell ref="B86:F86"/>
     <mergeCell ref="B97:F97"/>
     <mergeCell ref="B107:F107"/>
-    <mergeCell ref="B143:F143"/>
-    <mergeCell ref="B154:F154"/>
-    <mergeCell ref="B171:F171"/>
-    <mergeCell ref="B181:F181"/>
+    <mergeCell ref="B133:F133"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Started Integration for Orders
</commit_message>
<xml_diff>
--- a/Database Schema/Shopping_Database.xlsx
+++ b/Database Schema/Shopping_Database.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\eShoppingAdmin\Database Schema\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{161FE019-61D3-4F86-8297-96EF1F36E247}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1ACFFAD9-C803-4E1D-9674-08325F9B08FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{23AB6FBB-2C3C-4DC6-A36A-5E0C15916A1A}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="899" uniqueCount="181">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="895" uniqueCount="181">
   <si>
     <t>Users</t>
   </si>
@@ -566,9 +566,6 @@
     <t>ProductColorCode</t>
   </si>
   <si>
-    <t>ProductImageURL</t>
-  </si>
-  <si>
     <t>ProductPrice</t>
   </si>
   <si>
@@ -579,6 +576,9 @@
   </si>
   <si>
     <t>optional set of name of image</t>
+  </si>
+  <si>
+    <t>Date and Time when order is completed</t>
   </si>
 </sst>
 </file>
@@ -783,7 +783,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
@@ -802,6 +802,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1165,31 +1168,31 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:20" ht="18" x14ac:dyDescent="0.35">
-      <c r="B3" s="14" t="s">
+      <c r="B3" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="15"/>
-      <c r="D3" s="16"/>
-      <c r="F3" s="14" t="s">
+      <c r="C3" s="16"/>
+      <c r="D3" s="17"/>
+      <c r="F3" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="G3" s="15"/>
-      <c r="H3" s="16"/>
-      <c r="J3" s="14" t="s">
+      <c r="G3" s="16"/>
+      <c r="H3" s="17"/>
+      <c r="J3" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="K3" s="15"/>
-      <c r="L3" s="16"/>
-      <c r="N3" s="14" t="s">
+      <c r="K3" s="16"/>
+      <c r="L3" s="17"/>
+      <c r="N3" s="15" t="s">
         <v>49</v>
       </c>
-      <c r="O3" s="15"/>
-      <c r="P3" s="16"/>
-      <c r="R3" s="14" t="s">
+      <c r="O3" s="16"/>
+      <c r="P3" s="17"/>
+      <c r="R3" s="15" t="s">
         <v>55</v>
       </c>
-      <c r="S3" s="15"/>
-      <c r="T3" s="16"/>
+      <c r="S3" s="16"/>
+      <c r="T3" s="17"/>
     </row>
     <row r="4" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B4" s="1" t="s">
@@ -1356,11 +1359,11 @@
         <v>2</v>
       </c>
       <c r="D8" s="3"/>
-      <c r="F8" s="14" t="s">
+      <c r="F8" s="15" t="s">
         <v>45</v>
       </c>
-      <c r="G8" s="15"/>
-      <c r="H8" s="16"/>
+      <c r="G8" s="16"/>
+      <c r="H8" s="17"/>
       <c r="J8" s="4" t="s">
         <v>34</v>
       </c>
@@ -1512,11 +1515,11 @@
         <v>1</v>
       </c>
       <c r="P12" s="8"/>
-      <c r="R12" s="14" t="s">
+      <c r="R12" s="15" t="s">
         <v>59</v>
       </c>
-      <c r="S12" s="15"/>
-      <c r="T12" s="16"/>
+      <c r="S12" s="16"/>
+      <c r="T12" s="17"/>
     </row>
     <row r="13" spans="2:20" ht="18" x14ac:dyDescent="0.35">
       <c r="B13" s="4" t="s">
@@ -1526,16 +1529,16 @@
         <v>2</v>
       </c>
       <c r="D13" s="3"/>
-      <c r="F13" s="14" t="s">
+      <c r="F13" s="15" t="s">
         <v>46</v>
       </c>
-      <c r="G13" s="15"/>
-      <c r="H13" s="16"/>
-      <c r="J13" s="14" t="s">
+      <c r="G13" s="16"/>
+      <c r="H13" s="17"/>
+      <c r="J13" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="K13" s="15"/>
-      <c r="L13" s="16"/>
+      <c r="K13" s="16"/>
+      <c r="L13" s="17"/>
       <c r="R13" s="4" t="s">
         <v>11</v>
       </c>
@@ -1570,11 +1573,11 @@
       <c r="L14" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="N14" s="14" t="s">
+      <c r="N14" s="15" t="s">
         <v>73</v>
       </c>
-      <c r="O14" s="15"/>
-      <c r="P14" s="16"/>
+      <c r="O14" s="16"/>
+      <c r="P14" s="17"/>
       <c r="R14" s="4" t="s">
         <v>60</v>
       </c>
@@ -1622,11 +1625,11 @@
       </c>
     </row>
     <row r="16" spans="2:20" ht="18" x14ac:dyDescent="0.35">
-      <c r="B16" s="14" t="s">
+      <c r="B16" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="C16" s="15"/>
-      <c r="D16" s="16"/>
+      <c r="C16" s="16"/>
+      <c r="D16" s="17"/>
       <c r="J16" s="6" t="s">
         <v>37</v>
       </c>
@@ -1661,11 +1664,11 @@
       <c r="D17" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="F17" s="14" t="s">
+      <c r="F17" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="G17" s="15"/>
-      <c r="H17" s="16"/>
+      <c r="G17" s="16"/>
+      <c r="H17" s="17"/>
       <c r="N17" s="6" t="s">
         <v>35</v>
       </c>
@@ -1700,11 +1703,11 @@
         <v>1</v>
       </c>
       <c r="H18" s="3"/>
-      <c r="J18" s="14" t="s">
+      <c r="J18" s="15" t="s">
         <v>38</v>
       </c>
-      <c r="K18" s="15"/>
-      <c r="L18" s="16"/>
+      <c r="K18" s="16"/>
+      <c r="L18" s="17"/>
       <c r="R18" s="4" t="s">
         <v>32</v>
       </c>
@@ -1848,11 +1851,11 @@
         <v>43</v>
       </c>
       <c r="D24" s="8"/>
-      <c r="R24" s="14" t="s">
+      <c r="R24" s="15" t="s">
         <v>66</v>
       </c>
-      <c r="S24" s="15"/>
-      <c r="T24" s="16"/>
+      <c r="S24" s="16"/>
+      <c r="T24" s="17"/>
     </row>
     <row r="25" spans="2:20" x14ac:dyDescent="0.3">
       <c r="R25" s="4" t="s">
@@ -1866,11 +1869,11 @@
       </c>
     </row>
     <row r="26" spans="2:20" ht="18" x14ac:dyDescent="0.35">
-      <c r="B26" s="14" t="s">
+      <c r="B26" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="C26" s="15"/>
-      <c r="D26" s="16"/>
+      <c r="C26" s="16"/>
+      <c r="D26" s="17"/>
       <c r="R26" s="4" t="s">
         <v>60</v>
       </c>
@@ -1938,11 +1941,11 @@
       </c>
     </row>
     <row r="31" spans="2:20" ht="18" x14ac:dyDescent="0.35">
-      <c r="B31" s="14" t="s">
+      <c r="B31" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="C31" s="15"/>
-      <c r="D31" s="16"/>
+      <c r="C31" s="16"/>
+      <c r="D31" s="17"/>
     </row>
     <row r="32" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B32" s="4" t="s">
@@ -1966,6 +1969,11 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="R3:T3"/>
+    <mergeCell ref="R12:T12"/>
+    <mergeCell ref="R24:T24"/>
+    <mergeCell ref="B3:D3"/>
+    <mergeCell ref="B16:D16"/>
     <mergeCell ref="B31:D31"/>
     <mergeCell ref="B26:D26"/>
     <mergeCell ref="N14:P14"/>
@@ -1977,11 +1985,6 @@
     <mergeCell ref="F13:H13"/>
     <mergeCell ref="F17:H17"/>
     <mergeCell ref="N3:P3"/>
-    <mergeCell ref="R3:T3"/>
-    <mergeCell ref="R12:T12"/>
-    <mergeCell ref="R24:T24"/>
-    <mergeCell ref="B3:D3"/>
-    <mergeCell ref="B16:D16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1990,10 +1993,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE0C0E27-F398-4128-B7EC-E6C5B9DA9B0B}">
-  <dimension ref="B2:AE214"/>
+  <dimension ref="B2:AE213"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A109" workbookViewId="0">
-      <selection activeCell="H125" sqref="H125"/>
+    <sheetView tabSelected="1" topLeftCell="A163" workbookViewId="0">
+      <selection activeCell="C195" sqref="C195"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2006,22 +2009,22 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:6" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="18" t="s">
+      <c r="B2" s="19" t="s">
         <v>79</v>
       </c>
-      <c r="C2" s="19"/>
-      <c r="D2" s="19"/>
-      <c r="E2" s="19"/>
-      <c r="F2" s="20"/>
+      <c r="C2" s="20"/>
+      <c r="D2" s="20"/>
+      <c r="E2" s="20"/>
+      <c r="F2" s="21"/>
     </row>
     <row r="4" spans="2:6" ht="21" x14ac:dyDescent="0.4">
-      <c r="B4" s="17" t="s">
+      <c r="B4" s="18" t="s">
         <v>80</v>
       </c>
-      <c r="C4" s="17"/>
-      <c r="D4" s="17"/>
-      <c r="E4" s="17"/>
-      <c r="F4" s="17"/>
+      <c r="C4" s="18"/>
+      <c r="D4" s="18"/>
+      <c r="E4" s="18"/>
+      <c r="F4" s="18"/>
     </row>
     <row r="6" spans="2:6" ht="18" x14ac:dyDescent="0.35">
       <c r="B6" s="12" t="s">
@@ -2258,13 +2261,13 @@
       </c>
     </row>
     <row r="21" spans="2:7" ht="21" x14ac:dyDescent="0.4">
-      <c r="B21" s="17" t="s">
+      <c r="B21" s="18" t="s">
         <v>100</v>
       </c>
-      <c r="C21" s="17"/>
-      <c r="D21" s="17"/>
-      <c r="E21" s="17"/>
-      <c r="F21" s="17"/>
+      <c r="C21" s="18"/>
+      <c r="D21" s="18"/>
+      <c r="E21" s="18"/>
+      <c r="F21" s="18"/>
     </row>
     <row r="23" spans="2:7" ht="18" x14ac:dyDescent="0.35">
       <c r="B23" s="12" t="s">
@@ -2400,13 +2403,13 @@
       </c>
     </row>
     <row r="32" spans="2:7" ht="21" x14ac:dyDescent="0.4">
-      <c r="B32" s="17" t="s">
+      <c r="B32" s="18" t="s">
         <v>93</v>
       </c>
-      <c r="C32" s="17"/>
-      <c r="D32" s="17"/>
-      <c r="E32" s="17"/>
-      <c r="F32" s="17"/>
+      <c r="C32" s="18"/>
+      <c r="D32" s="18"/>
+      <c r="E32" s="18"/>
+      <c r="F32" s="18"/>
     </row>
     <row r="34" spans="2:6" ht="18" x14ac:dyDescent="0.35">
       <c r="B34" s="12" t="s">
@@ -2592,13 +2595,13 @@
       </c>
     </row>
     <row r="46" spans="2:6" ht="21" x14ac:dyDescent="0.4">
-      <c r="B46" s="17" t="s">
+      <c r="B46" s="18" t="s">
         <v>154</v>
       </c>
-      <c r="C46" s="17"/>
-      <c r="D46" s="17"/>
-      <c r="E46" s="17"/>
-      <c r="F46" s="17"/>
+      <c r="C46" s="18"/>
+      <c r="D46" s="18"/>
+      <c r="E46" s="18"/>
+      <c r="F46" s="18"/>
     </row>
     <row r="48" spans="2:6" ht="18" x14ac:dyDescent="0.35">
       <c r="B48" s="12" t="s">
@@ -2733,13 +2736,13 @@
       </c>
     </row>
     <row r="57" spans="2:31" ht="21" x14ac:dyDescent="0.4">
-      <c r="B57" s="17" t="s">
+      <c r="B57" s="18" t="s">
         <v>102</v>
       </c>
-      <c r="C57" s="17"/>
-      <c r="D57" s="17"/>
-      <c r="E57" s="17"/>
-      <c r="F57" s="17"/>
+      <c r="C57" s="18"/>
+      <c r="D57" s="18"/>
+      <c r="E57" s="18"/>
+      <c r="F57" s="18"/>
       <c r="AE57" s="10"/>
     </row>
     <row r="59" spans="2:31" ht="18" x14ac:dyDescent="0.35">
@@ -2858,13 +2861,13 @@
       </c>
     </row>
     <row r="67" spans="2:31" ht="21" x14ac:dyDescent="0.4">
-      <c r="B67" s="17" t="s">
+      <c r="B67" s="18" t="s">
         <v>105</v>
       </c>
-      <c r="C67" s="17"/>
-      <c r="D67" s="17"/>
-      <c r="E67" s="17"/>
-      <c r="F67" s="17"/>
+      <c r="C67" s="18"/>
+      <c r="D67" s="18"/>
+      <c r="E67" s="18"/>
+      <c r="F67" s="18"/>
       <c r="AE67" s="10"/>
     </row>
     <row r="69" spans="2:31" ht="18" x14ac:dyDescent="0.35">
@@ -2966,13 +2969,13 @@
       </c>
     </row>
     <row r="76" spans="2:31" ht="21" x14ac:dyDescent="0.4">
-      <c r="B76" s="17" t="s">
+      <c r="B76" s="18" t="s">
         <v>107</v>
       </c>
-      <c r="C76" s="17"/>
-      <c r="D76" s="17"/>
-      <c r="E76" s="17"/>
-      <c r="F76" s="17"/>
+      <c r="C76" s="18"/>
+      <c r="D76" s="18"/>
+      <c r="E76" s="18"/>
+      <c r="F76" s="18"/>
       <c r="AE76" s="10"/>
     </row>
     <row r="78" spans="2:31" ht="18" x14ac:dyDescent="0.35">
@@ -3098,13 +3101,13 @@
     </row>
     <row r="85" spans="2:31" ht="16.2" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="86" spans="2:31" ht="21" x14ac:dyDescent="0.4">
-      <c r="B86" s="17" t="s">
+      <c r="B86" s="18" t="s">
         <v>109</v>
       </c>
-      <c r="C86" s="17"/>
-      <c r="D86" s="17"/>
-      <c r="E86" s="17"/>
-      <c r="F86" s="17"/>
+      <c r="C86" s="18"/>
+      <c r="D86" s="18"/>
+      <c r="E86" s="18"/>
+      <c r="F86" s="18"/>
     </row>
     <row r="88" spans="2:31" ht="18" x14ac:dyDescent="0.35">
       <c r="B88" s="12" t="s">
@@ -3247,13 +3250,13 @@
       <c r="F96" s="5"/>
     </row>
     <row r="97" spans="2:31" ht="21" x14ac:dyDescent="0.4">
-      <c r="B97" s="17" t="s">
+      <c r="B97" s="18" t="s">
         <v>111</v>
       </c>
-      <c r="C97" s="17"/>
-      <c r="D97" s="17"/>
-      <c r="E97" s="17"/>
-      <c r="F97" s="17"/>
+      <c r="C97" s="18"/>
+      <c r="D97" s="18"/>
+      <c r="E97" s="18"/>
+      <c r="F97" s="18"/>
     </row>
     <row r="99" spans="2:31" ht="18" x14ac:dyDescent="0.35">
       <c r="B99" s="12" t="s">
@@ -3372,13 +3375,13 @@
       </c>
     </row>
     <row r="107" spans="2:31" ht="21" x14ac:dyDescent="0.4">
-      <c r="B107" s="17" t="s">
+      <c r="B107" s="18" t="s">
         <v>112</v>
       </c>
-      <c r="C107" s="17"/>
-      <c r="D107" s="17"/>
-      <c r="E107" s="17"/>
-      <c r="F107" s="17"/>
+      <c r="C107" s="18"/>
+      <c r="D107" s="18"/>
+      <c r="E107" s="18"/>
+      <c r="F107" s="18"/>
       <c r="AE107" s="10"/>
     </row>
     <row r="108" spans="2:31" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -3481,13 +3484,13 @@
       </c>
     </row>
     <row r="116" spans="2:31" ht="21" x14ac:dyDescent="0.4">
-      <c r="B116" s="17" t="s">
+      <c r="B116" s="18" t="s">
         <v>114</v>
       </c>
-      <c r="C116" s="17"/>
-      <c r="D116" s="17"/>
-      <c r="E116" s="17"/>
-      <c r="F116" s="17"/>
+      <c r="C116" s="18"/>
+      <c r="D116" s="18"/>
+      <c r="E116" s="18"/>
+      <c r="F116" s="18"/>
     </row>
     <row r="118" spans="2:31" ht="18" x14ac:dyDescent="0.35">
       <c r="B118" s="12" t="s">
@@ -3560,7 +3563,7 @@
     </row>
     <row r="122" spans="2:31" x14ac:dyDescent="0.3">
       <c r="B122" s="5" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C122" s="5" t="s">
         <v>1</v>
@@ -3614,14 +3617,14 @@
         <v>36</v>
       </c>
       <c r="C125" s="9" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D125" s="11"/>
       <c r="E125" s="9" t="s">
         <v>81</v>
       </c>
       <c r="F125" s="9" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="126" spans="2:31" x14ac:dyDescent="0.3">
@@ -3660,7 +3663,7 @@
     </row>
     <row r="128" spans="2:31" x14ac:dyDescent="0.3">
       <c r="B128" s="9" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C128" s="9" t="s">
         <v>1</v>
@@ -3724,13 +3727,13 @@
       </c>
     </row>
     <row r="133" spans="2:31" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B133" s="17" t="s">
+      <c r="B133" s="18" t="s">
         <v>117</v>
       </c>
-      <c r="C133" s="17"/>
-      <c r="D133" s="17"/>
-      <c r="E133" s="17"/>
-      <c r="F133" s="17"/>
+      <c r="C133" s="18"/>
+      <c r="D133" s="18"/>
+      <c r="E133" s="18"/>
+      <c r="F133" s="18"/>
     </row>
     <row r="135" spans="2:31" ht="18" x14ac:dyDescent="0.35">
       <c r="B135" s="12" t="s">
@@ -3866,13 +3869,13 @@
       </c>
     </row>
     <row r="144" spans="2:31" ht="21" x14ac:dyDescent="0.4">
-      <c r="B144" s="17" t="s">
+      <c r="B144" s="18" t="s">
         <v>119</v>
       </c>
-      <c r="C144" s="17"/>
-      <c r="D144" s="17"/>
-      <c r="E144" s="17"/>
-      <c r="F144" s="17"/>
+      <c r="C144" s="18"/>
+      <c r="D144" s="18"/>
+      <c r="E144" s="18"/>
+      <c r="F144" s="18"/>
     </row>
     <row r="146" spans="2:31" ht="18" x14ac:dyDescent="0.35">
       <c r="B146" s="12" t="s">
@@ -4110,13 +4113,13 @@
       </c>
     </row>
     <row r="161" spans="2:31" ht="21" x14ac:dyDescent="0.4">
-      <c r="B161" s="17" t="s">
+      <c r="B161" s="18" t="s">
         <v>120</v>
       </c>
-      <c r="C161" s="17"/>
-      <c r="D161" s="17"/>
-      <c r="E161" s="17"/>
-      <c r="F161" s="17"/>
+      <c r="C161" s="18"/>
+      <c r="D161" s="18"/>
+      <c r="E161" s="18"/>
+      <c r="F161" s="18"/>
     </row>
     <row r="162" spans="2:31" x14ac:dyDescent="0.3">
       <c r="AE162" s="10"/>
@@ -4238,13 +4241,13 @@
       </c>
     </row>
     <row r="171" spans="2:31" ht="21" x14ac:dyDescent="0.4">
-      <c r="B171" s="17" t="s">
+      <c r="B171" s="18" t="s">
         <v>121</v>
       </c>
-      <c r="C171" s="17"/>
-      <c r="D171" s="17"/>
-      <c r="E171" s="17"/>
-      <c r="F171" s="17"/>
+      <c r="C171" s="18"/>
+      <c r="D171" s="18"/>
+      <c r="E171" s="18"/>
+      <c r="F171" s="18"/>
     </row>
     <row r="173" spans="2:31" ht="18" x14ac:dyDescent="0.35">
       <c r="B173" s="12" t="s">
@@ -4300,22 +4303,24 @@
     </row>
     <row r="176" spans="2:31" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B176" s="5" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C176" s="5" t="s">
-        <v>91</v>
-      </c>
-      <c r="D176" s="11"/>
+        <v>1</v>
+      </c>
+      <c r="D176" s="11">
+        <v>11</v>
+      </c>
       <c r="E176" s="5" t="s">
         <v>81</v>
       </c>
       <c r="F176" s="5" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
     </row>
     <row r="177" spans="2:31" x14ac:dyDescent="0.3">
       <c r="B177" s="5" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C177" s="5" t="s">
         <v>1</v>
@@ -4332,51 +4337,49 @@
     </row>
     <row r="178" spans="2:31" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B178" s="5" t="s">
-        <v>58</v>
+        <v>67</v>
       </c>
       <c r="C178" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="D178" s="11">
-        <v>11</v>
-      </c>
+        <v>91</v>
+      </c>
+      <c r="D178" s="11"/>
       <c r="E178" s="5" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="F178" s="5" t="s">
-        <v>115</v>
+        <v>180</v>
       </c>
     </row>
     <row r="179" spans="2:31" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B179" s="5" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C179" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="D179" s="11"/>
+        <v>3</v>
+      </c>
+      <c r="D179" s="11">
+        <v>11</v>
+      </c>
       <c r="E179" s="5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F179" s="5" t="s">
-        <v>115</v>
+        <v>123</v>
       </c>
     </row>
     <row r="180" spans="2:31" x14ac:dyDescent="0.3">
       <c r="B180" s="5" t="s">
-        <v>65</v>
+        <v>130</v>
       </c>
       <c r="C180" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="D180" s="11">
-        <v>11</v>
-      </c>
+        <v>91</v>
+      </c>
+      <c r="D180" s="11"/>
       <c r="E180" s="5" t="s">
         <v>81</v>
       </c>
       <c r="F180" s="5" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="181" spans="2:31" x14ac:dyDescent="0.3">
@@ -4412,13 +4415,13 @@
       </c>
     </row>
     <row r="184" spans="2:31" ht="21" x14ac:dyDescent="0.4">
-      <c r="B184" s="17" t="s">
+      <c r="B184" s="18" t="s">
         <v>124</v>
       </c>
-      <c r="C184" s="17"/>
-      <c r="D184" s="17"/>
-      <c r="E184" s="17"/>
-      <c r="F184" s="17"/>
+      <c r="C184" s="18"/>
+      <c r="D184" s="18"/>
+      <c r="E184" s="18"/>
+      <c r="F184" s="18"/>
     </row>
     <row r="186" spans="2:31" ht="18" x14ac:dyDescent="0.35">
       <c r="B186" s="12" t="s">
@@ -4525,13 +4528,13 @@
     </row>
     <row r="192" spans="2:31" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B192" s="5" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="C192" s="5" t="s">
         <v>2</v>
       </c>
       <c r="D192" s="11">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="E192" s="5" t="s">
         <v>81</v>
@@ -4541,25 +4544,25 @@
       </c>
     </row>
     <row r="193" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B193" s="5" t="s">
-        <v>173</v>
-      </c>
-      <c r="C193" s="5" t="s">
+      <c r="B193" s="9" t="s">
+        <v>174</v>
+      </c>
+      <c r="C193" s="9" t="s">
         <v>2</v>
       </c>
       <c r="D193" s="11">
         <v>50</v>
       </c>
-      <c r="E193" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="F193" s="5" t="s">
+      <c r="E193" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="F193" s="9" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="194" spans="2:6" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B194" s="9" t="s">
-        <v>174</v>
+    <row r="194" spans="2:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B194" s="5" t="s">
+        <v>175</v>
       </c>
       <c r="C194" s="9" t="s">
         <v>2</v>
@@ -4567,22 +4570,22 @@
       <c r="D194" s="11">
         <v>50</v>
       </c>
-      <c r="E194" s="9" t="s">
-        <v>81</v>
-      </c>
-      <c r="F194" s="9" t="s">
+      <c r="E194" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="F194" s="5" t="s">
         <v>115</v>
       </c>
     </row>
     <row r="195" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B195" s="5" t="s">
-        <v>175</v>
-      </c>
-      <c r="C195" s="9" t="s">
-        <v>2</v>
+        <v>62</v>
+      </c>
+      <c r="C195" s="5" t="s">
+        <v>1</v>
       </c>
       <c r="D195" s="11">
-        <v>50</v>
+        <v>11</v>
       </c>
       <c r="E195" s="5" t="s">
         <v>81</v>
@@ -4593,7 +4596,7 @@
     </row>
     <row r="196" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B196" s="5" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C196" s="5" t="s">
         <v>1</v>
@@ -4610,7 +4613,7 @@
     </row>
     <row r="197" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B197" s="5" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="C197" s="5" t="s">
         <v>1</v>
@@ -4626,25 +4629,23 @@
       </c>
     </row>
     <row r="198" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B198" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="C198" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="D198" s="11">
-        <v>11</v>
-      </c>
-      <c r="E198" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="F198" s="5" t="s">
-        <v>115</v>
+      <c r="B198" s="9" t="s">
+        <v>130</v>
+      </c>
+      <c r="C198" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="D198" s="11"/>
+      <c r="E198" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="F198" s="9" t="s">
+        <v>145</v>
       </c>
     </row>
     <row r="199" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B199" s="9" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="C199" s="9" t="s">
         <v>91</v>
@@ -4654,70 +4655,72 @@
         <v>82</v>
       </c>
       <c r="F199" s="9" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="200" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B200" s="9" t="s">
-        <v>128</v>
+        <v>83</v>
       </c>
       <c r="C200" s="9" t="s">
-        <v>91</v>
-      </c>
-      <c r="D200" s="11"/>
-      <c r="E200" s="9" t="s">
-        <v>82</v>
-      </c>
-      <c r="F200" s="9" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="201" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B201" s="9" t="s">
-        <v>83</v>
-      </c>
-      <c r="C201" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="D201" s="11">
-        <v>2</v>
-      </c>
-      <c r="E201" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="F201" s="5" t="s">
+      <c r="D200" s="11">
+        <v>2</v>
+      </c>
+      <c r="E200" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="F200" s="5" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="203" spans="2:6" ht="21" x14ac:dyDescent="0.4">
-      <c r="B203" s="17" t="s">
+    <row r="202" spans="2:6" ht="21" x14ac:dyDescent="0.4">
+      <c r="B202" s="14" t="s">
         <v>125</v>
       </c>
-      <c r="C203" s="17"/>
-      <c r="D203" s="17"/>
-      <c r="E203" s="17"/>
-      <c r="F203" s="17"/>
-    </row>
-    <row r="205" spans="2:6" ht="18" x14ac:dyDescent="0.35">
-      <c r="B205" s="12" t="s">
+      <c r="C202" s="14"/>
+      <c r="D202" s="14"/>
+      <c r="E202" s="14"/>
+      <c r="F202" s="14"/>
+    </row>
+    <row r="204" spans="2:6" ht="18" x14ac:dyDescent="0.35">
+      <c r="B204" s="12" t="s">
         <v>74</v>
       </c>
-      <c r="C205" s="12" t="s">
+      <c r="C204" s="12" t="s">
         <v>75</v>
       </c>
-      <c r="D205" s="13" t="s">
+      <c r="D204" s="13" t="s">
         <v>76</v>
       </c>
-      <c r="E205" s="12" t="s">
+      <c r="E204" s="12" t="s">
         <v>77</v>
       </c>
-      <c r="F205" s="12" t="s">
+      <c r="F204" s="12" t="s">
         <v>78</v>
+      </c>
+    </row>
+    <row r="205" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B205" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C205" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="D205" s="11">
+        <v>11</v>
+      </c>
+      <c r="E205" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="F205" s="5" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="206" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B206" s="5" t="s">
-        <v>11</v>
+        <v>60</v>
       </c>
       <c r="C206" s="5" t="s">
         <v>1</v>
@@ -4729,46 +4732,46 @@
         <v>81</v>
       </c>
       <c r="F206" s="5" t="s">
-        <v>84</v>
+        <v>116</v>
       </c>
     </row>
     <row r="207" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B207" s="5" t="s">
-        <v>60</v>
+        <v>20</v>
       </c>
       <c r="C207" s="5" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D207" s="11">
-        <v>11</v>
+        <v>50</v>
       </c>
       <c r="E207" s="5" t="s">
         <v>81</v>
       </c>
       <c r="F207" s="5" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="208" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B208" s="5" t="s">
-        <v>20</v>
+        <v>151</v>
       </c>
       <c r="C208" s="5" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D208" s="11">
-        <v>50</v>
+        <v>11</v>
       </c>
       <c r="E208" s="5" t="s">
         <v>81</v>
       </c>
       <c r="F208" s="5" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
     </row>
     <row r="209" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B209" s="5" t="s">
-        <v>151</v>
+        <v>22</v>
       </c>
       <c r="C209" s="5" t="s">
         <v>1</v>
@@ -4785,7 +4788,7 @@
     </row>
     <row r="210" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B210" s="5" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C210" s="5" t="s">
         <v>1</v>
@@ -4801,25 +4804,23 @@
       </c>
     </row>
     <row r="211" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B211" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="C211" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="D211" s="11">
-        <v>11</v>
-      </c>
-      <c r="E211" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="F211" s="5" t="s">
-        <v>116</v>
+      <c r="B211" s="9" t="s">
+        <v>130</v>
+      </c>
+      <c r="C211" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="D211" s="11"/>
+      <c r="E211" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="F211" s="9" t="s">
+        <v>146</v>
       </c>
     </row>
     <row r="212" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B212" s="9" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="C212" s="9" t="s">
         <v>91</v>
@@ -4829,60 +4830,44 @@
         <v>82</v>
       </c>
       <c r="F212" s="9" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
     </row>
     <row r="213" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B213" s="9" t="s">
-        <v>128</v>
+        <v>83</v>
       </c>
       <c r="C213" s="9" t="s">
-        <v>91</v>
-      </c>
-      <c r="D213" s="11"/>
-      <c r="E213" s="9" t="s">
-        <v>82</v>
-      </c>
-      <c r="F213" s="9" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="214" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B214" s="9" t="s">
-        <v>83</v>
-      </c>
-      <c r="C214" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="D214" s="11">
-        <v>2</v>
-      </c>
-      <c r="E214" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="F214" s="5" t="s">
+      <c r="D213" s="11">
+        <v>2</v>
+      </c>
+      <c r="E213" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="F213" s="5" t="s">
         <v>149</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="18">
-    <mergeCell ref="B144:F144"/>
-    <mergeCell ref="B161:F161"/>
-    <mergeCell ref="B171:F171"/>
-    <mergeCell ref="B203:F203"/>
-    <mergeCell ref="B21:F21"/>
+  <mergeCells count="17">
     <mergeCell ref="B2:F2"/>
     <mergeCell ref="B4:F4"/>
     <mergeCell ref="B32:F32"/>
     <mergeCell ref="B57:F57"/>
     <mergeCell ref="B116:F116"/>
-    <mergeCell ref="B184:F184"/>
     <mergeCell ref="B46:F46"/>
     <mergeCell ref="B67:F67"/>
     <mergeCell ref="B76:F76"/>
     <mergeCell ref="B86:F86"/>
     <mergeCell ref="B97:F97"/>
     <mergeCell ref="B107:F107"/>
+    <mergeCell ref="B144:F144"/>
+    <mergeCell ref="B161:F161"/>
+    <mergeCell ref="B171:F171"/>
+    <mergeCell ref="B21:F21"/>
+    <mergeCell ref="B184:F184"/>
     <mergeCell ref="B133:F133"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added new Orders Page for displaying all orders and make it index.php page dynamic
</commit_message>
<xml_diff>
--- a/Database Schema/Shopping_Database.xlsx
+++ b/Database Schema/Shopping_Database.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\eShoppingAdmin\Database Schema\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1ACFFAD9-C803-4E1D-9674-08325F9B08FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B04647EA-8A79-447A-B298-DF55DF28652E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{23AB6FBB-2C3C-4DC6-A36A-5E0C15916A1A}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="895" uniqueCount="181">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="891" uniqueCount="180">
   <si>
     <t>Users</t>
   </si>
@@ -576,9 +576,6 @@
   </si>
   <si>
     <t>optional set of name of image</t>
-  </si>
-  <si>
-    <t>Date and Time when order is completed</t>
   </si>
 </sst>
 </file>
@@ -816,9 +813,6 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -827,6 +821,9 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1969,11 +1966,6 @@
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="R3:T3"/>
-    <mergeCell ref="R12:T12"/>
-    <mergeCell ref="R24:T24"/>
-    <mergeCell ref="B3:D3"/>
-    <mergeCell ref="B16:D16"/>
     <mergeCell ref="B31:D31"/>
     <mergeCell ref="B26:D26"/>
     <mergeCell ref="N14:P14"/>
@@ -1985,6 +1977,11 @@
     <mergeCell ref="F13:H13"/>
     <mergeCell ref="F17:H17"/>
     <mergeCell ref="N3:P3"/>
+    <mergeCell ref="R3:T3"/>
+    <mergeCell ref="R12:T12"/>
+    <mergeCell ref="R24:T24"/>
+    <mergeCell ref="B3:D3"/>
+    <mergeCell ref="B16:D16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1993,10 +1990,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE0C0E27-F398-4128-B7EC-E6C5B9DA9B0B}">
-  <dimension ref="B2:AE213"/>
+  <dimension ref="B2:AE212"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A163" workbookViewId="0">
-      <selection activeCell="C195" sqref="C195"/>
+    <sheetView tabSelected="1" topLeftCell="A187" workbookViewId="0">
+      <selection activeCell="G186" sqref="G186"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2009,22 +2006,22 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:6" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="19" t="s">
+      <c r="B2" s="18" t="s">
         <v>79</v>
       </c>
-      <c r="C2" s="20"/>
-      <c r="D2" s="20"/>
-      <c r="E2" s="20"/>
-      <c r="F2" s="21"/>
+      <c r="C2" s="19"/>
+      <c r="D2" s="19"/>
+      <c r="E2" s="19"/>
+      <c r="F2" s="20"/>
     </row>
     <row r="4" spans="2:6" ht="21" x14ac:dyDescent="0.4">
-      <c r="B4" s="18" t="s">
+      <c r="B4" s="21" t="s">
         <v>80</v>
       </c>
-      <c r="C4" s="18"/>
-      <c r="D4" s="18"/>
-      <c r="E4" s="18"/>
-      <c r="F4" s="18"/>
+      <c r="C4" s="21"/>
+      <c r="D4" s="21"/>
+      <c r="E4" s="21"/>
+      <c r="F4" s="21"/>
     </row>
     <row r="6" spans="2:6" ht="18" x14ac:dyDescent="0.35">
       <c r="B6" s="12" t="s">
@@ -2261,13 +2258,13 @@
       </c>
     </row>
     <row r="21" spans="2:7" ht="21" x14ac:dyDescent="0.4">
-      <c r="B21" s="18" t="s">
+      <c r="B21" s="21" t="s">
         <v>100</v>
       </c>
-      <c r="C21" s="18"/>
-      <c r="D21" s="18"/>
-      <c r="E21" s="18"/>
-      <c r="F21" s="18"/>
+      <c r="C21" s="21"/>
+      <c r="D21" s="21"/>
+      <c r="E21" s="21"/>
+      <c r="F21" s="21"/>
     </row>
     <row r="23" spans="2:7" ht="18" x14ac:dyDescent="0.35">
       <c r="B23" s="12" t="s">
@@ -2403,13 +2400,13 @@
       </c>
     </row>
     <row r="32" spans="2:7" ht="21" x14ac:dyDescent="0.4">
-      <c r="B32" s="18" t="s">
+      <c r="B32" s="21" t="s">
         <v>93</v>
       </c>
-      <c r="C32" s="18"/>
-      <c r="D32" s="18"/>
-      <c r="E32" s="18"/>
-      <c r="F32" s="18"/>
+      <c r="C32" s="21"/>
+      <c r="D32" s="21"/>
+      <c r="E32" s="21"/>
+      <c r="F32" s="21"/>
     </row>
     <row r="34" spans="2:6" ht="18" x14ac:dyDescent="0.35">
       <c r="B34" s="12" t="s">
@@ -2595,13 +2592,13 @@
       </c>
     </row>
     <row r="46" spans="2:6" ht="21" x14ac:dyDescent="0.4">
-      <c r="B46" s="18" t="s">
+      <c r="B46" s="21" t="s">
         <v>154</v>
       </c>
-      <c r="C46" s="18"/>
-      <c r="D46" s="18"/>
-      <c r="E46" s="18"/>
-      <c r="F46" s="18"/>
+      <c r="C46" s="21"/>
+      <c r="D46" s="21"/>
+      <c r="E46" s="21"/>
+      <c r="F46" s="21"/>
     </row>
     <row r="48" spans="2:6" ht="18" x14ac:dyDescent="0.35">
       <c r="B48" s="12" t="s">
@@ -2736,13 +2733,13 @@
       </c>
     </row>
     <row r="57" spans="2:31" ht="21" x14ac:dyDescent="0.4">
-      <c r="B57" s="18" t="s">
+      <c r="B57" s="21" t="s">
         <v>102</v>
       </c>
-      <c r="C57" s="18"/>
-      <c r="D57" s="18"/>
-      <c r="E57" s="18"/>
-      <c r="F57" s="18"/>
+      <c r="C57" s="21"/>
+      <c r="D57" s="21"/>
+      <c r="E57" s="21"/>
+      <c r="F57" s="21"/>
       <c r="AE57" s="10"/>
     </row>
     <row r="59" spans="2:31" ht="18" x14ac:dyDescent="0.35">
@@ -2861,13 +2858,13 @@
       </c>
     </row>
     <row r="67" spans="2:31" ht="21" x14ac:dyDescent="0.4">
-      <c r="B67" s="18" t="s">
+      <c r="B67" s="21" t="s">
         <v>105</v>
       </c>
-      <c r="C67" s="18"/>
-      <c r="D67" s="18"/>
-      <c r="E67" s="18"/>
-      <c r="F67" s="18"/>
+      <c r="C67" s="21"/>
+      <c r="D67" s="21"/>
+      <c r="E67" s="21"/>
+      <c r="F67" s="21"/>
       <c r="AE67" s="10"/>
     </row>
     <row r="69" spans="2:31" ht="18" x14ac:dyDescent="0.35">
@@ -2969,13 +2966,13 @@
       </c>
     </row>
     <row r="76" spans="2:31" ht="21" x14ac:dyDescent="0.4">
-      <c r="B76" s="18" t="s">
+      <c r="B76" s="21" t="s">
         <v>107</v>
       </c>
-      <c r="C76" s="18"/>
-      <c r="D76" s="18"/>
-      <c r="E76" s="18"/>
-      <c r="F76" s="18"/>
+      <c r="C76" s="21"/>
+      <c r="D76" s="21"/>
+      <c r="E76" s="21"/>
+      <c r="F76" s="21"/>
       <c r="AE76" s="10"/>
     </row>
     <row r="78" spans="2:31" ht="18" x14ac:dyDescent="0.35">
@@ -3101,13 +3098,13 @@
     </row>
     <row r="85" spans="2:31" ht="16.2" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="86" spans="2:31" ht="21" x14ac:dyDescent="0.4">
-      <c r="B86" s="18" t="s">
+      <c r="B86" s="21" t="s">
         <v>109</v>
       </c>
-      <c r="C86" s="18"/>
-      <c r="D86" s="18"/>
-      <c r="E86" s="18"/>
-      <c r="F86" s="18"/>
+      <c r="C86" s="21"/>
+      <c r="D86" s="21"/>
+      <c r="E86" s="21"/>
+      <c r="F86" s="21"/>
     </row>
     <row r="88" spans="2:31" ht="18" x14ac:dyDescent="0.35">
       <c r="B88" s="12" t="s">
@@ -3250,13 +3247,13 @@
       <c r="F96" s="5"/>
     </row>
     <row r="97" spans="2:31" ht="21" x14ac:dyDescent="0.4">
-      <c r="B97" s="18" t="s">
+      <c r="B97" s="21" t="s">
         <v>111</v>
       </c>
-      <c r="C97" s="18"/>
-      <c r="D97" s="18"/>
-      <c r="E97" s="18"/>
-      <c r="F97" s="18"/>
+      <c r="C97" s="21"/>
+      <c r="D97" s="21"/>
+      <c r="E97" s="21"/>
+      <c r="F97" s="21"/>
     </row>
     <row r="99" spans="2:31" ht="18" x14ac:dyDescent="0.35">
       <c r="B99" s="12" t="s">
@@ -3375,13 +3372,13 @@
       </c>
     </row>
     <row r="107" spans="2:31" ht="21" x14ac:dyDescent="0.4">
-      <c r="B107" s="18" t="s">
+      <c r="B107" s="21" t="s">
         <v>112</v>
       </c>
-      <c r="C107" s="18"/>
-      <c r="D107" s="18"/>
-      <c r="E107" s="18"/>
-      <c r="F107" s="18"/>
+      <c r="C107" s="21"/>
+      <c r="D107" s="21"/>
+      <c r="E107" s="21"/>
+      <c r="F107" s="21"/>
       <c r="AE107" s="10"/>
     </row>
     <row r="108" spans="2:31" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -3484,13 +3481,13 @@
       </c>
     </row>
     <row r="116" spans="2:31" ht="21" x14ac:dyDescent="0.4">
-      <c r="B116" s="18" t="s">
+      <c r="B116" s="21" t="s">
         <v>114</v>
       </c>
-      <c r="C116" s="18"/>
-      <c r="D116" s="18"/>
-      <c r="E116" s="18"/>
-      <c r="F116" s="18"/>
+      <c r="C116" s="21"/>
+      <c r="D116" s="21"/>
+      <c r="E116" s="21"/>
+      <c r="F116" s="21"/>
     </row>
     <row r="118" spans="2:31" ht="18" x14ac:dyDescent="0.35">
       <c r="B118" s="12" t="s">
@@ -3727,13 +3724,13 @@
       </c>
     </row>
     <row r="133" spans="2:31" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B133" s="18" t="s">
+      <c r="B133" s="21" t="s">
         <v>117</v>
       </c>
-      <c r="C133" s="18"/>
-      <c r="D133" s="18"/>
-      <c r="E133" s="18"/>
-      <c r="F133" s="18"/>
+      <c r="C133" s="21"/>
+      <c r="D133" s="21"/>
+      <c r="E133" s="21"/>
+      <c r="F133" s="21"/>
     </row>
     <row r="135" spans="2:31" ht="18" x14ac:dyDescent="0.35">
       <c r="B135" s="12" t="s">
@@ -3869,13 +3866,13 @@
       </c>
     </row>
     <row r="144" spans="2:31" ht="21" x14ac:dyDescent="0.4">
-      <c r="B144" s="18" t="s">
+      <c r="B144" s="21" t="s">
         <v>119</v>
       </c>
-      <c r="C144" s="18"/>
-      <c r="D144" s="18"/>
-      <c r="E144" s="18"/>
-      <c r="F144" s="18"/>
+      <c r="C144" s="21"/>
+      <c r="D144" s="21"/>
+      <c r="E144" s="21"/>
+      <c r="F144" s="21"/>
     </row>
     <row r="146" spans="2:31" ht="18" x14ac:dyDescent="0.35">
       <c r="B146" s="12" t="s">
@@ -4113,13 +4110,13 @@
       </c>
     </row>
     <row r="161" spans="2:31" ht="21" x14ac:dyDescent="0.4">
-      <c r="B161" s="18" t="s">
+      <c r="B161" s="21" t="s">
         <v>120</v>
       </c>
-      <c r="C161" s="18"/>
-      <c r="D161" s="18"/>
-      <c r="E161" s="18"/>
-      <c r="F161" s="18"/>
+      <c r="C161" s="21"/>
+      <c r="D161" s="21"/>
+      <c r="E161" s="21"/>
+      <c r="F161" s="21"/>
     </row>
     <row r="162" spans="2:31" x14ac:dyDescent="0.3">
       <c r="AE162" s="10"/>
@@ -4241,13 +4238,13 @@
       </c>
     </row>
     <row r="171" spans="2:31" ht="21" x14ac:dyDescent="0.4">
-      <c r="B171" s="18" t="s">
+      <c r="B171" s="21" t="s">
         <v>121</v>
       </c>
-      <c r="C171" s="18"/>
-      <c r="D171" s="18"/>
-      <c r="E171" s="18"/>
-      <c r="F171" s="18"/>
+      <c r="C171" s="21"/>
+      <c r="D171" s="21"/>
+      <c r="E171" s="21"/>
+      <c r="F171" s="21"/>
     </row>
     <row r="173" spans="2:31" ht="18" x14ac:dyDescent="0.35">
       <c r="B173" s="12" t="s">
@@ -4337,112 +4334,114 @@
     </row>
     <row r="178" spans="2:31" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B178" s="5" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C178" s="5" t="s">
-        <v>91</v>
-      </c>
-      <c r="D178" s="11"/>
+        <v>3</v>
+      </c>
+      <c r="D178" s="11">
+        <v>11</v>
+      </c>
       <c r="E178" s="5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F178" s="5" t="s">
-        <v>180</v>
+        <v>123</v>
       </c>
     </row>
     <row r="179" spans="2:31" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B179" s="5" t="s">
-        <v>65</v>
+        <v>130</v>
       </c>
       <c r="C179" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="D179" s="11">
-        <v>11</v>
-      </c>
+        <v>91</v>
+      </c>
+      <c r="D179" s="11"/>
       <c r="E179" s="5" t="s">
         <v>81</v>
       </c>
       <c r="F179" s="5" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="180" spans="2:31" x14ac:dyDescent="0.3">
-      <c r="B180" s="5" t="s">
-        <v>130</v>
-      </c>
-      <c r="C180" s="5" t="s">
+      <c r="B180" s="9" t="s">
+        <v>128</v>
+      </c>
+      <c r="C180" s="9" t="s">
         <v>91</v>
       </c>
       <c r="D180" s="11"/>
-      <c r="E180" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="F180" s="5" t="s">
-        <v>122</v>
+      <c r="E180" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="F180" s="9" t="s">
+        <v>143</v>
       </c>
     </row>
     <row r="181" spans="2:31" x14ac:dyDescent="0.3">
       <c r="B181" s="9" t="s">
-        <v>128</v>
+        <v>83</v>
       </c>
       <c r="C181" s="9" t="s">
-        <v>91</v>
-      </c>
-      <c r="D181" s="11"/>
-      <c r="E181" s="9" t="s">
-        <v>82</v>
-      </c>
-      <c r="F181" s="9" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="182" spans="2:31" x14ac:dyDescent="0.3">
-      <c r="B182" s="9" t="s">
-        <v>83</v>
-      </c>
-      <c r="C182" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="D182" s="11">
-        <v>2</v>
-      </c>
-      <c r="E182" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="F182" s="5" t="s">
+      <c r="D181" s="11">
+        <v>2</v>
+      </c>
+      <c r="E181" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="F181" s="5" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="184" spans="2:31" ht="21" x14ac:dyDescent="0.4">
-      <c r="B184" s="18" t="s">
+    <row r="183" spans="2:31" ht="21" x14ac:dyDescent="0.4">
+      <c r="B183" s="14" t="s">
         <v>124</v>
       </c>
-      <c r="C184" s="18"/>
-      <c r="D184" s="18"/>
-      <c r="E184" s="18"/>
-      <c r="F184" s="18"/>
-    </row>
-    <row r="186" spans="2:31" ht="18" x14ac:dyDescent="0.35">
-      <c r="B186" s="12" t="s">
+      <c r="C183" s="14"/>
+      <c r="D183" s="14"/>
+      <c r="E183" s="14"/>
+      <c r="F183" s="14"/>
+    </row>
+    <row r="185" spans="2:31" ht="18" x14ac:dyDescent="0.35">
+      <c r="B185" s="12" t="s">
         <v>74</v>
       </c>
-      <c r="C186" s="12" t="s">
+      <c r="C185" s="12" t="s">
         <v>75</v>
       </c>
-      <c r="D186" s="13" t="s">
+      <c r="D185" s="13" t="s">
         <v>76</v>
       </c>
-      <c r="E186" s="12" t="s">
+      <c r="E185" s="12" t="s">
         <v>77</v>
       </c>
-      <c r="F186" s="12" t="s">
+      <c r="F185" s="12" t="s">
         <v>78</v>
+      </c>
+    </row>
+    <row r="186" spans="2:31" x14ac:dyDescent="0.3">
+      <c r="B186" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C186" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="D186" s="11">
+        <v>11</v>
+      </c>
+      <c r="E186" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="F186" s="5" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="187" spans="2:31" x14ac:dyDescent="0.3">
       <c r="B187" s="5" t="s">
-        <v>11</v>
+        <v>60</v>
       </c>
       <c r="C187" s="5" t="s">
         <v>1</v>
@@ -4454,12 +4453,12 @@
         <v>81</v>
       </c>
       <c r="F187" s="5" t="s">
-        <v>84</v>
+        <v>116</v>
       </c>
     </row>
     <row r="188" spans="2:31" x14ac:dyDescent="0.3">
       <c r="B188" s="5" t="s">
-        <v>60</v>
+        <v>35</v>
       </c>
       <c r="C188" s="5" t="s">
         <v>1</v>
@@ -4476,24 +4475,24 @@
     </row>
     <row r="189" spans="2:31" x14ac:dyDescent="0.3">
       <c r="B189" s="5" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="C189" s="5" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D189" s="11">
-        <v>11</v>
+        <v>50</v>
       </c>
       <c r="E189" s="5" t="s">
         <v>81</v>
       </c>
       <c r="F189" s="5" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="190" spans="2:31" x14ac:dyDescent="0.3">
       <c r="B190" s="5" t="s">
-        <v>29</v>
+        <v>61</v>
       </c>
       <c r="C190" s="5" t="s">
         <v>2</v>
@@ -4511,7 +4510,7 @@
     </row>
     <row r="191" spans="2:31" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B191" s="5" t="s">
-        <v>61</v>
+        <v>173</v>
       </c>
       <c r="C191" s="5" t="s">
         <v>2</v>
@@ -4527,25 +4526,25 @@
       </c>
     </row>
     <row r="192" spans="2:31" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B192" s="5" t="s">
-        <v>173</v>
-      </c>
-      <c r="C192" s="5" t="s">
+      <c r="B192" s="9" t="s">
+        <v>174</v>
+      </c>
+      <c r="C192" s="9" t="s">
         <v>2</v>
       </c>
       <c r="D192" s="11">
         <v>50</v>
       </c>
-      <c r="E192" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="F192" s="5" t="s">
+      <c r="E192" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="F192" s="9" t="s">
         <v>115</v>
       </c>
     </row>
     <row r="193" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B193" s="9" t="s">
-        <v>174</v>
+      <c r="B193" s="5" t="s">
+        <v>175</v>
       </c>
       <c r="C193" s="9" t="s">
         <v>2</v>
@@ -4553,22 +4552,22 @@
       <c r="D193" s="11">
         <v>50</v>
       </c>
-      <c r="E193" s="9" t="s">
-        <v>81</v>
-      </c>
-      <c r="F193" s="9" t="s">
+      <c r="E193" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="F193" s="5" t="s">
         <v>115</v>
       </c>
     </row>
     <row r="194" spans="2:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B194" s="5" t="s">
-        <v>175</v>
-      </c>
-      <c r="C194" s="9" t="s">
-        <v>2</v>
+        <v>62</v>
+      </c>
+      <c r="C194" s="5" t="s">
+        <v>1</v>
       </c>
       <c r="D194" s="11">
-        <v>50</v>
+        <v>11</v>
       </c>
       <c r="E194" s="5" t="s">
         <v>81</v>
@@ -4579,7 +4578,7 @@
     </row>
     <row r="195" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B195" s="5" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C195" s="5" t="s">
         <v>1</v>
@@ -4596,7 +4595,7 @@
     </row>
     <row r="196" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B196" s="5" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="C196" s="5" t="s">
         <v>1</v>
@@ -4612,25 +4611,23 @@
       </c>
     </row>
     <row r="197" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B197" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="C197" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="D197" s="11">
-        <v>11</v>
-      </c>
-      <c r="E197" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="F197" s="5" t="s">
-        <v>115</v>
+      <c r="B197" s="9" t="s">
+        <v>130</v>
+      </c>
+      <c r="C197" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="D197" s="11"/>
+      <c r="E197" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="F197" s="9" t="s">
+        <v>145</v>
       </c>
     </row>
     <row r="198" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B198" s="9" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="C198" s="9" t="s">
         <v>91</v>
@@ -4640,70 +4637,72 @@
         <v>82</v>
       </c>
       <c r="F198" s="9" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="199" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B199" s="9" t="s">
-        <v>128</v>
+        <v>83</v>
       </c>
       <c r="C199" s="9" t="s">
-        <v>91</v>
-      </c>
-      <c r="D199" s="11"/>
-      <c r="E199" s="9" t="s">
-        <v>82</v>
-      </c>
-      <c r="F199" s="9" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="200" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B200" s="9" t="s">
-        <v>83</v>
-      </c>
-      <c r="C200" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="D200" s="11">
-        <v>2</v>
-      </c>
-      <c r="E200" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="F200" s="5" t="s">
+      <c r="D199" s="11">
+        <v>2</v>
+      </c>
+      <c r="E199" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="F199" s="5" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="202" spans="2:6" ht="21" x14ac:dyDescent="0.4">
-      <c r="B202" s="14" t="s">
+    <row r="201" spans="2:6" ht="21" x14ac:dyDescent="0.4">
+      <c r="B201" s="14" t="s">
         <v>125</v>
       </c>
-      <c r="C202" s="14"/>
-      <c r="D202" s="14"/>
-      <c r="E202" s="14"/>
-      <c r="F202" s="14"/>
-    </row>
-    <row r="204" spans="2:6" ht="18" x14ac:dyDescent="0.35">
-      <c r="B204" s="12" t="s">
+      <c r="C201" s="14"/>
+      <c r="D201" s="14"/>
+      <c r="E201" s="14"/>
+      <c r="F201" s="14"/>
+    </row>
+    <row r="203" spans="2:6" ht="18" x14ac:dyDescent="0.35">
+      <c r="B203" s="12" t="s">
         <v>74</v>
       </c>
-      <c r="C204" s="12" t="s">
+      <c r="C203" s="12" t="s">
         <v>75</v>
       </c>
-      <c r="D204" s="13" t="s">
+      <c r="D203" s="13" t="s">
         <v>76</v>
       </c>
-      <c r="E204" s="12" t="s">
+      <c r="E203" s="12" t="s">
         <v>77</v>
       </c>
-      <c r="F204" s="12" t="s">
+      <c r="F203" s="12" t="s">
         <v>78</v>
+      </c>
+    </row>
+    <row r="204" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B204" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C204" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="D204" s="11">
+        <v>11</v>
+      </c>
+      <c r="E204" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="F204" s="5" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="205" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B205" s="5" t="s">
-        <v>11</v>
+        <v>60</v>
       </c>
       <c r="C205" s="5" t="s">
         <v>1</v>
@@ -4715,46 +4714,46 @@
         <v>81</v>
       </c>
       <c r="F205" s="5" t="s">
-        <v>84</v>
+        <v>116</v>
       </c>
     </row>
     <row r="206" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B206" s="5" t="s">
-        <v>60</v>
+        <v>20</v>
       </c>
       <c r="C206" s="5" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D206" s="11">
-        <v>11</v>
+        <v>50</v>
       </c>
       <c r="E206" s="5" t="s">
         <v>81</v>
       </c>
       <c r="F206" s="5" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="207" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B207" s="5" t="s">
-        <v>20</v>
+        <v>151</v>
       </c>
       <c r="C207" s="5" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D207" s="11">
-        <v>50</v>
+        <v>11</v>
       </c>
       <c r="E207" s="5" t="s">
         <v>81</v>
       </c>
       <c r="F207" s="5" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
     </row>
     <row r="208" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B208" s="5" t="s">
-        <v>151</v>
+        <v>22</v>
       </c>
       <c r="C208" s="5" t="s">
         <v>1</v>
@@ -4771,7 +4770,7 @@
     </row>
     <row r="209" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B209" s="5" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C209" s="5" t="s">
         <v>1</v>
@@ -4787,25 +4786,23 @@
       </c>
     </row>
     <row r="210" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B210" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="C210" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="D210" s="11">
-        <v>11</v>
-      </c>
-      <c r="E210" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="F210" s="5" t="s">
-        <v>116</v>
+      <c r="B210" s="9" t="s">
+        <v>130</v>
+      </c>
+      <c r="C210" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="D210" s="11"/>
+      <c r="E210" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="F210" s="9" t="s">
+        <v>146</v>
       </c>
     </row>
     <row r="211" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B211" s="9" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="C211" s="9" t="s">
         <v>91</v>
@@ -4815,43 +4812,33 @@
         <v>82</v>
       </c>
       <c r="F211" s="9" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
     </row>
     <row r="212" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B212" s="9" t="s">
-        <v>128</v>
+        <v>83</v>
       </c>
       <c r="C212" s="9" t="s">
-        <v>91</v>
-      </c>
-      <c r="D212" s="11"/>
-      <c r="E212" s="9" t="s">
-        <v>82</v>
-      </c>
-      <c r="F212" s="9" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="213" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B213" s="9" t="s">
-        <v>83</v>
-      </c>
-      <c r="C213" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="D213" s="11">
-        <v>2</v>
-      </c>
-      <c r="E213" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="F213" s="5" t="s">
+      <c r="D212" s="11">
+        <v>2</v>
+      </c>
+      <c r="E212" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="F212" s="5" t="s">
         <v>149</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="17">
+  <mergeCells count="16">
+    <mergeCell ref="B144:F144"/>
+    <mergeCell ref="B161:F161"/>
+    <mergeCell ref="B171:F171"/>
+    <mergeCell ref="B21:F21"/>
+    <mergeCell ref="B133:F133"/>
     <mergeCell ref="B2:F2"/>
     <mergeCell ref="B4:F4"/>
     <mergeCell ref="B32:F32"/>
@@ -4863,12 +4850,6 @@
     <mergeCell ref="B86:F86"/>
     <mergeCell ref="B97:F97"/>
     <mergeCell ref="B107:F107"/>
-    <mergeCell ref="B144:F144"/>
-    <mergeCell ref="B161:F161"/>
-    <mergeCell ref="B171:F171"/>
-    <mergeCell ref="B21:F21"/>
-    <mergeCell ref="B184:F184"/>
-    <mergeCell ref="B133:F133"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>